<commit_message>
Adding in training_data.csv file and looking to create a scoring mechanism.
</commit_message>
<xml_diff>
--- a/what_to_wear_outdoors/data/What I wore running.xlsx
+++ b/what_to_wear_outdoors/data/What I wore running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c10a0a3541b6f8b5/Fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="9" documentId="6_{2B9A42AB-0138-4469-A0A8-F8E64854B08E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{542D2FF2-3962-4ECD-826E-5A60DA9B95C2}"/>
+  <xr:revisionPtr revIDLastSave="37" documentId="6_{2B9A42AB-0138-4469-A0A8-F8E64854B08E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9F1AF645-A4EC-49C4-A5A6-52ACAA2798C0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="8976" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1323" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="182">
   <si>
     <t>Run</t>
   </si>
@@ -964,8 +964,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y31" totalsRowShown="0">
-  <autoFilter ref="A1:Y31" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y33" totalsRowShown="0">
+  <autoFilter ref="A1:Y33" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y26">
     <sortCondition ref="B1:B26"/>
   </sortState>
@@ -1399,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC4919-1670-4AFD-91C3-CDFEF0B7A9A5}">
-  <dimension ref="A1:AB31"/>
+  <dimension ref="A1:AB33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="X2" sqref="X2:X31"/>
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>1</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="AB4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="AB5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>37</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -3763,12 +3763,101 @@
         <v>29</v>
       </c>
     </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>43</v>
+      </c>
+      <c r="B32" s="1">
+        <v>43456</v>
+      </c>
+      <c r="C32" s="4">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D32" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E32" s="5">
+        <v>7</v>
+      </c>
+      <c r="F32" s="6">
+        <v>70</v>
+      </c>
+      <c r="G32" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H32" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I32" s="5">
+        <v>10</v>
+      </c>
+      <c r="J32" s="5" t="s">
+        <v>177</v>
+      </c>
+      <c r="K32" s="5">
+        <v>36</v>
+      </c>
+      <c r="L32" s="5">
+        <v>29</v>
+      </c>
+      <c r="M32" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="N32" s="7"/>
+      <c r="O32" s="2"/>
+      <c r="P32" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q32" t="s">
+        <v>163</v>
+      </c>
+      <c r="R32" t="s">
+        <v>157</v>
+      </c>
+      <c r="S32" t="s">
+        <v>29</v>
+      </c>
+      <c r="T32" t="s">
+        <v>157</v>
+      </c>
+      <c r="U32" t="s">
+        <v>30</v>
+      </c>
+      <c r="V32" t="s">
+        <v>172</v>
+      </c>
+      <c r="W32" t="s">
+        <v>29</v>
+      </c>
+      <c r="X32" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
+      <c r="B33" s="1"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="6"/>
+      <c r="G33" s="6"/>
+      <c r="H33" s="5"/>
+      <c r="I33" s="5"/>
+      <c r="J33" s="5"/>
+      <c r="K33" s="5"/>
+      <c r="L33" s="5"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="2"/>
+    </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G31" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G33" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
       <formula1>Conditions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T31" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T33" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
       <formula1>JacketOption</formula1>
     </dataValidation>
   </dataValidations>
@@ -3784,25 +3873,25 @@
           <x14:formula1>
             <xm:f>ValidValues!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P31 S2:S31 U2:U31 W2:W31 Y2:Y31</xm:sqref>
+          <xm:sqref>P2:P33 S2:S33 U2:U33 W2:W33 Y2:Y33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BFEBF07-64B2-450B-BC13-447B52D5D711}">
           <x14:formula1>
             <xm:f>ValidValues!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:R31</xm:sqref>
+          <xm:sqref>Q2:R33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E09EE0F-16F0-4536-B318-2F013ED3F6AB}">
           <x14:formula1>
             <xm:f>ValidValues!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V31</xm:sqref>
+          <xm:sqref>V2:V33</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1617D946-B125-4BE6-B340-3AE6EE661815}">
           <x14:formula1>
             <xm:f>ValidValues!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X31</xm:sqref>
+          <xm:sqref>X2:X33</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4096,7 +4185,7 @@
       </c>
       <c r="AF3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>91</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -4190,7 +4279,7 @@
       </c>
       <c r="AF4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>17</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -4284,7 +4373,7 @@
       </c>
       <c r="AF5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>36</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added a config.py file to keep up with the "constants". Moved models out of the predictors in order to use the 'strategy' pattern to try and improve the models without breaking the predictors. Added a mode to generate data so that that would be a starting point to have training data. Decided to keep the xlsx sheet around just for the actuals in order to score the models. Added a mechanism to score models
</commit_message>
<xml_diff>
--- a/what_to_wear_outdoors/data/What I wore running.xlsx
+++ b/what_to_wear_outdoors/data/What I wore running.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c10a0a3541b6f8b5/Fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="37" documentId="6_{2B9A42AB-0138-4469-A0A8-F8E64854B08E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{9F1AF645-A4EC-49C4-A5A6-52ACAA2798C0}"/>
+  <xr:revisionPtr revIDLastSave="56" documentId="6_{AD7A7900-7A15-4D12-BB88-955DD6692745}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3B88C80B-4537-4054-9A21-EC1B0159303E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="30696" windowHeight="8976" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="8976" activeTab="2" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log2" sheetId="5" r:id="rId1"/>
@@ -21,7 +21,7 @@
   </sheets>
   <definedNames>
     <definedName name="Conditions">ValidValues!$A$2:$A$94</definedName>
-    <definedName name="JacketOption">ValidValues!$H$2:$H$9</definedName>
+    <definedName name="JacketOption">ValidValues!$H$2:$H$10</definedName>
     <definedName name="LabelOptions">Table6[Layer]</definedName>
     <definedName name="LayerOptions">Table6[Layer]</definedName>
     <definedName name="LegOptions">Table410[Legs]</definedName>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1338" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="182">
   <si>
     <t>Run</t>
   </si>
@@ -549,18 +549,6 @@
     <t>Rain-Wind</t>
   </si>
   <si>
-    <t>Warmth</t>
-  </si>
-  <si>
-    <t>Warmth-Rain</t>
-  </si>
-  <si>
-    <t>Warmth-Wind</t>
-  </si>
-  <si>
-    <t>Warmth-Rain-Wind</t>
-  </si>
-  <si>
     <t>Base Layer</t>
   </si>
   <si>
@@ -592,6 +580,18 @@
   </si>
   <si>
     <t>Boot</t>
+  </si>
+  <si>
+    <t>Vest</t>
+  </si>
+  <si>
+    <t>Warm-Rain</t>
+  </si>
+  <si>
+    <t>Warm-Wind</t>
+  </si>
+  <si>
+    <t>Warm-Rain-Wind</t>
   </si>
 </sst>
 </file>
@@ -964,8 +964,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y33" totalsRowShown="0">
-  <autoFilter ref="A1:Y33" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y35" totalsRowShown="0">
+  <autoFilter ref="A1:Y35" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y26">
     <sortCondition ref="B1:B26"/>
   </sortState>
@@ -1082,8 +1082,8 @@
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFA7AAA-B2FF-4D4A-BCAA-9C4A9B7254BE}" name="Table7" displayName="Table7" ref="H1:H9" totalsRowShown="0">
-  <autoFilter ref="H1:H9" xr:uid="{CDE8C1FF-4045-47A3-8733-EC2F500BE5ED}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{CDFA7AAA-B2FF-4D4A-BCAA-9C4A9B7254BE}" name="Table7" displayName="Table7" ref="H1:H10" totalsRowShown="0">
+  <autoFilter ref="H1:H10" xr:uid="{CDE8C1FF-4045-47A3-8733-EC2F500BE5ED}"/>
   <tableColumns count="1">
     <tableColumn id="1" xr3:uid="{C30292A7-7B6D-498C-BA45-4B72A9BB1A31}" name="Jacket"/>
   </tableColumns>
@@ -1399,10 +1399,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC4919-1670-4AFD-91C3-CDFEF0B7A9A5}">
-  <dimension ref="A1:AB33"/>
+  <dimension ref="A1:AB35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A33" sqref="A33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1466,13 +1466,13 @@
         <v>26</v>
       </c>
       <c r="P1" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="Q1" t="s">
         <v>159</v>
       </c>
       <c r="R1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -1484,7 +1484,7 @@
         <v>19</v>
       </c>
       <c r="V1" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="W1" t="s">
         <v>24</v>
@@ -1559,7 +1559,7 @@
         <v>29</v>
       </c>
       <c r="V2" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W2" t="s">
         <v>29</v>
@@ -1634,7 +1634,7 @@
         <v>29</v>
       </c>
       <c r="V3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W3" t="s">
         <v>38</v>
@@ -1650,7 +1650,7 @@
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>51</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1732,7 +1732,7 @@
       </c>
       <c r="AB4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1814,7 +1814,7 @@
       </c>
       <c r="AB5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>65</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1957,7 +1957,7 @@
         <v>29</v>
       </c>
       <c r="V7" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W7" t="s">
         <v>38</v>
@@ -2032,7 +2032,7 @@
         <v>30</v>
       </c>
       <c r="V8" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W8" t="s">
         <v>38</v>
@@ -2182,7 +2182,7 @@
         <v>30</v>
       </c>
       <c r="V10" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W10" t="s">
         <v>29</v>
@@ -2257,7 +2257,7 @@
         <v>30</v>
       </c>
       <c r="V11" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W11" t="s">
         <v>38</v>
@@ -2332,7 +2332,7 @@
         <v>30</v>
       </c>
       <c r="V12" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W12" t="s">
         <v>38</v>
@@ -2409,7 +2409,7 @@
         <v>30</v>
       </c>
       <c r="V13" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W13" t="s">
         <v>38</v>
@@ -2484,7 +2484,7 @@
         <v>30</v>
       </c>
       <c r="V14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W14" t="s">
         <v>38</v>
@@ -2559,7 +2559,7 @@
         <v>30</v>
       </c>
       <c r="V15" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W15" t="s">
         <v>38</v>
@@ -2634,7 +2634,7 @@
         <v>29</v>
       </c>
       <c r="V16" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W16" t="s">
         <v>38</v>
@@ -2784,7 +2784,7 @@
         <v>30</v>
       </c>
       <c r="V18" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W18" t="s">
         <v>38</v>
@@ -2936,7 +2936,7 @@
         <v>30</v>
       </c>
       <c r="V20" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W20" t="s">
         <v>29</v>
@@ -3232,7 +3232,7 @@
         <v>29</v>
       </c>
       <c r="V24" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W24" t="s">
         <v>29</v>
@@ -3305,7 +3305,7 @@
         <v>30</v>
       </c>
       <c r="V25" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W25" t="s">
         <v>29</v>
@@ -3380,7 +3380,7 @@
         <v>30</v>
       </c>
       <c r="V26" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W26" t="s">
         <v>29</v>
@@ -3455,7 +3455,7 @@
         <v>29</v>
       </c>
       <c r="V27" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="W27" t="s">
         <v>29</v>
@@ -3530,7 +3530,7 @@
         <v>30</v>
       </c>
       <c r="V28" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W28" t="s">
         <v>30</v>
@@ -3605,7 +3605,7 @@
         <v>29</v>
       </c>
       <c r="V29" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W29" t="s">
         <v>29</v>
@@ -3678,7 +3678,7 @@
         <v>29</v>
       </c>
       <c r="V30" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W30" t="s">
         <v>38</v>
@@ -3719,7 +3719,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -3751,7 +3751,7 @@
         <v>30</v>
       </c>
       <c r="V31" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W31" t="s">
         <v>38</v>
@@ -3792,7 +3792,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K32" s="5">
         <v>36</v>
@@ -3824,7 +3824,7 @@
         <v>30</v>
       </c>
       <c r="V32" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="W32" t="s">
         <v>29</v>
@@ -3836,28 +3836,174 @@
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="2:15" x14ac:dyDescent="0.3">
-      <c r="B33" s="1"/>
-      <c r="C33" s="4"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="6"/>
-      <c r="G33" s="6"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="7"/>
+    <row r="33" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>43</v>
+      </c>
+      <c r="B33" s="1">
+        <v>43458</v>
+      </c>
+      <c r="C33" s="4">
+        <v>0.3125</v>
+      </c>
+      <c r="D33" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E33" s="5">
+        <v>6</v>
+      </c>
+      <c r="F33" s="6">
+        <v>70</v>
+      </c>
+      <c r="G33" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H33" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I33" s="5">
+        <v>0</v>
+      </c>
+      <c r="J33" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K33" s="5">
+        <v>27</v>
+      </c>
+      <c r="L33" s="5">
+        <v>27</v>
+      </c>
+      <c r="M33" s="7">
+        <v>0.93</v>
+      </c>
       <c r="N33" s="7"/>
       <c r="O33" s="2"/>
+      <c r="P33" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>157</v>
+      </c>
+      <c r="R33" t="s">
+        <v>163</v>
+      </c>
+      <c r="S33" t="s">
+        <v>29</v>
+      </c>
+      <c r="T33" t="s">
+        <v>178</v>
+      </c>
+      <c r="U33" t="s">
+        <v>30</v>
+      </c>
+      <c r="V33" t="s">
+        <v>168</v>
+      </c>
+      <c r="W33" t="s">
+        <v>30</v>
+      </c>
+      <c r="X33" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>43</v>
+      </c>
+      <c r="B34" s="1">
+        <v>43461</v>
+      </c>
+      <c r="C34" s="4">
+        <v>0.35416666666666669</v>
+      </c>
+      <c r="D34" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E34" s="5">
+        <v>3</v>
+      </c>
+      <c r="F34" s="6">
+        <v>30</v>
+      </c>
+      <c r="G34" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H34" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I34" s="5">
+        <v>13</v>
+      </c>
+      <c r="J34" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K34" s="5">
+        <v>54</v>
+      </c>
+      <c r="L34" s="5">
+        <v>54</v>
+      </c>
+      <c r="M34" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="N34" s="7"/>
+      <c r="O34" s="2"/>
+      <c r="P34" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q34" t="s">
+        <v>157</v>
+      </c>
+      <c r="R34" t="s">
+        <v>163</v>
+      </c>
+      <c r="S34" t="s">
+        <v>29</v>
+      </c>
+      <c r="T34" t="s">
+        <v>157</v>
+      </c>
+      <c r="U34" t="s">
+        <v>29</v>
+      </c>
+      <c r="V34" t="s">
+        <v>20</v>
+      </c>
+      <c r="W34" t="s">
+        <v>29</v>
+      </c>
+      <c r="X34" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="35" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B35" s="1"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="6"/>
+      <c r="G35" s="6"/>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+      <c r="J35" s="5"/>
+      <c r="K35" s="5"/>
+      <c r="L35" s="5"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G33" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
       <formula1>Conditions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T33" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T35" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
       <formula1>JacketOption</formula1>
     </dataValidation>
   </dataValidations>
@@ -3873,25 +4019,25 @@
           <x14:formula1>
             <xm:f>ValidValues!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P33 S2:S33 U2:U33 W2:W33 Y2:Y33</xm:sqref>
+          <xm:sqref>P2:P35 S2:S35 U2:U35 W2:W35 Y2:Y35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BFEBF07-64B2-450B-BC13-447B52D5D711}">
           <x14:formula1>
             <xm:f>ValidValues!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:R33</xm:sqref>
+          <xm:sqref>Q2:R35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E09EE0F-16F0-4536-B318-2F013ED3F6AB}">
           <x14:formula1>
             <xm:f>ValidValues!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V33</xm:sqref>
+          <xm:sqref>V2:V35</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1617D946-B125-4BE6-B340-3AE6EE661815}">
           <x14:formula1>
             <xm:f>ValidValues!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X33</xm:sqref>
+          <xm:sqref>X2:X35</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4185,7 +4331,7 @@
       </c>
       <c r="AF3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>23</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -4279,7 +4425,7 @@
       </c>
       <c r="AF4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>2</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -4373,7 +4519,7 @@
       </c>
       <c r="AF5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>61</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -6578,7 +6724,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -6686,8 +6832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF5CF31-5DCF-45F0-99A9-605CADC9A594}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6716,10 +6862,10 @@
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="J1" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6759,13 +6905,13 @@
         <v>160</v>
       </c>
       <c r="H3" t="s">
-        <v>165</v>
+        <v>178</v>
       </c>
       <c r="I3" t="s">
-        <v>175</v>
+        <v>171</v>
       </c>
       <c r="J3" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -6779,13 +6925,13 @@
         <v>162</v>
       </c>
       <c r="H4" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="I4" t="s">
         <v>154</v>
       </c>
       <c r="J4" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
@@ -6799,10 +6945,10 @@
         <v>163</v>
       </c>
       <c r="H5" t="s">
-        <v>8</v>
+        <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
@@ -6813,10 +6959,10 @@
         <v>164</v>
       </c>
       <c r="H6" t="s">
-        <v>166</v>
+        <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
@@ -6824,7 +6970,7 @@
         <v>95</v>
       </c>
       <c r="H7" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
@@ -6832,7 +6978,7 @@
         <v>79</v>
       </c>
       <c r="H8" t="s">
-        <v>169</v>
+        <v>179</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
@@ -6840,13 +6986,16 @@
         <v>81</v>
       </c>
       <c r="H9" t="s">
-        <v>170</v>
+        <v>180</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>137</v>
       </c>
+      <c r="H10" t="s">
+        <v>181</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
@@ -7308,8 +7457,8 @@
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:A96">
-    <sortCondition ref="A96"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A6:A97">
+    <sortCondition ref="A97"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>

<commit_message>
Update of what I wore, with newest data.
</commit_message>
<xml_diff>
--- a/what_to_wear_outdoors/data/What I wore running.xlsx
+++ b/what_to_wear_outdoors/data/What I wore running.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c10a0a3541b6f8b5/Fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="56" documentId="6_{AD7A7900-7A15-4D12-BB88-955DD6692745}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{3B88C80B-4537-4054-9A21-EC1B0159303E}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="104_{AECD96ED-7C4A-43C3-A65D-5FA5035B2AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4560FAD1-0D85-4DD7-80A1-E79495EA9D66}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20640" windowHeight="8976" activeTab="2" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="3360" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
   </bookViews>
   <sheets>
     <sheet name="Activity Log2" sheetId="5" r:id="rId1"/>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1369" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="184">
   <si>
     <t>Run</t>
   </si>
@@ -592,6 +592,12 @@
   </si>
   <si>
     <t>Warm-Rain-Wind</t>
+  </si>
+  <si>
+    <t>NNE</t>
+  </si>
+  <si>
+    <t>Too warm</t>
   </si>
 </sst>
 </file>
@@ -964,8 +970,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y35" totalsRowShown="0">
-  <autoFilter ref="A1:Y35" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y36" totalsRowShown="0">
+  <autoFilter ref="A1:Y36" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y26">
     <sortCondition ref="B1:B26"/>
   </sortState>
@@ -1399,10 +1405,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC4919-1670-4AFD-91C3-CDFEF0B7A9A5}">
-  <dimension ref="A1:AB35"/>
+  <dimension ref="A1:AB36"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A35" sqref="A35"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1650,7 +1656,7 @@
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>48</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1732,7 +1738,7 @@
       </c>
       <c r="AB4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>4</v>
+        <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1814,7 +1820,7 @@
       </c>
       <c r="AB5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>38</v>
+        <v>52</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -3983,27 +3989,102 @@
       </c>
     </row>
     <row r="35" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B35" s="1"/>
-      <c r="C35" s="4"/>
-      <c r="D35" s="5"/>
-      <c r="E35" s="5"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="6"/>
-      <c r="H35" s="5"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="5"/>
-      <c r="K35" s="5"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="7"/>
-      <c r="N35" s="7"/>
+      <c r="A35" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" s="1">
+        <v>43463</v>
+      </c>
+      <c r="C35" s="4">
+        <v>0.30208333333333331</v>
+      </c>
+      <c r="D35" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E35" s="5">
+        <v>4</v>
+      </c>
+      <c r="F35" s="6">
+        <v>40</v>
+      </c>
+      <c r="G35" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H35" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I35" s="5">
+        <v>9</v>
+      </c>
+      <c r="J35" s="5" t="s">
+        <v>182</v>
+      </c>
+      <c r="K35" s="5">
+        <v>25</v>
+      </c>
+      <c r="L35" s="5">
+        <v>25</v>
+      </c>
+      <c r="M35" s="7">
+        <v>0.8</v>
+      </c>
+      <c r="N35" s="7" t="s">
+        <v>183</v>
+      </c>
       <c r="O35" s="2"/>
+      <c r="P35" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q35" t="s">
+        <v>164</v>
+      </c>
+      <c r="R35" t="s">
+        <v>163</v>
+      </c>
+      <c r="S35" t="s">
+        <v>29</v>
+      </c>
+      <c r="T35" t="s">
+        <v>157</v>
+      </c>
+      <c r="U35" t="s">
+        <v>30</v>
+      </c>
+      <c r="V35" t="s">
+        <v>168</v>
+      </c>
+      <c r="W35" t="s">
+        <v>38</v>
+      </c>
+      <c r="X35" t="s">
+        <v>157</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="36" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B36" s="1"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="5"/>
+      <c r="I36" s="5"/>
+      <c r="J36" s="5"/>
+      <c r="K36" s="5"/>
+      <c r="L36" s="5"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G35" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G36" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
       <formula1>Conditions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T35" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T36" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
       <formula1>JacketOption</formula1>
     </dataValidation>
   </dataValidations>
@@ -4019,25 +4100,25 @@
           <x14:formula1>
             <xm:f>ValidValues!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P35 S2:S35 U2:U35 W2:W35 Y2:Y35</xm:sqref>
+          <xm:sqref>P2:P36 S2:S36 U2:U36 W2:W36 Y2:Y36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BFEBF07-64B2-450B-BC13-447B52D5D711}">
           <x14:formula1>
             <xm:f>ValidValues!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:R35</xm:sqref>
+          <xm:sqref>Q2:R36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E09EE0F-16F0-4536-B318-2F013ED3F6AB}">
           <x14:formula1>
             <xm:f>ValidValues!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V35</xm:sqref>
+          <xm:sqref>V2:V36</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1617D946-B125-4BE6-B340-3AE6EE661815}">
           <x14:formula1>
             <xm:f>ValidValues!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X35</xm:sqref>
+          <xm:sqref>X2:X36</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4331,7 +4412,7 @@
       </c>
       <c r="AF3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -4425,7 +4506,7 @@
       </c>
       <c r="AF4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -4519,7 +4600,7 @@
       </c>
       <c r="AF5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>37</v>
+        <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -6832,7 +6913,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF5CF31-5DCF-45F0-99A9-605CADC9A594}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Extend ddt to accept categories other than light/dark
</commit_message>
<xml_diff>
--- a/what_to_wear_outdoors/data/What I wore running.xlsx
+++ b/what_to_wear_outdoors/data/What I wore running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c10a0a3541b6f8b5/Fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="104_{AECD96ED-7C4A-43C3-A65D-5FA5035B2AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4560FAD1-0D85-4DD7-80A1-E79495EA9D66}"/>
+  <xr:revisionPtr revIDLastSave="106" documentId="104_{AECD96ED-7C4A-43C3-A65D-5FA5035B2AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{2825A1B8-97E6-4330-B3B4-C5386AFE4EC0}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="3360" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="187">
   <si>
     <t>Run</t>
   </si>
@@ -240,240 +240,15 @@
     <t>Heavy Drizzel</t>
   </si>
   <si>
-    <t>Light  Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Rain</t>
-  </si>
-  <si>
     <t>Light  Snow</t>
   </si>
   <si>
-    <t>Heavy  Snow</t>
-  </si>
-  <si>
-    <t>Light  Snow Grains</t>
-  </si>
-  <si>
-    <t>Heavy  Snow Grains</t>
-  </si>
-  <si>
-    <t>Light  Ice Crystals</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Crystals</t>
-  </si>
-  <si>
-    <t>Light  Ice Pellets</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Pellets</t>
-  </si>
-  <si>
-    <t>Light  Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Hail</t>
-  </si>
-  <si>
     <t>Light  Mist</t>
   </si>
   <si>
-    <t>Heavy  Mist</t>
-  </si>
-  <si>
-    <t>Light  Fog</t>
-  </si>
-  <si>
-    <t>Heavy  Fog</t>
-  </si>
-  <si>
-    <t>Light  Fog Patches</t>
-  </si>
-  <si>
-    <t>Heavy  Fog Patches</t>
-  </si>
-  <si>
-    <t>Light  Smoke</t>
-  </si>
-  <si>
-    <t>Heavy  Smoke</t>
-  </si>
-  <si>
-    <t>Light  Volcanic Ash</t>
-  </si>
-  <si>
-    <t>Heavy  Volcanic Ash</t>
-  </si>
-  <si>
-    <t>Light  Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Sand</t>
-  </si>
-  <si>
-    <t>Light  Haze</t>
-  </si>
-  <si>
-    <t>Heavy  Haze</t>
-  </si>
-  <si>
-    <t>Light  Spray</t>
-  </si>
-  <si>
-    <t>Heavy  Spray</t>
-  </si>
-  <si>
-    <t>Light  Dust Whirls</t>
-  </si>
-  <si>
-    <t>Heavy  Dust Whirls</t>
-  </si>
-  <si>
-    <t>Light  Sandstorm</t>
-  </si>
-  <si>
-    <t>Heavy  Sandstorm</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Snow</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Sand</t>
-  </si>
-  <si>
-    <t>Light  Blowing Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Snow</t>
-  </si>
-  <si>
-    <t>Light  Blowing Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Blowing Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Sand</t>
-  </si>
-  <si>
-    <t>Light  Rain Mist</t>
-  </si>
-  <si>
-    <t>Heavy  Rain Mist</t>
-  </si>
-  <si>
-    <t>Light  Rain Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Rain Showers</t>
-  </si>
-  <si>
-    <t>Light  Snow Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Snow Showers</t>
-  </si>
-  <si>
     <t>Light  Snow Blowing Snow Mist</t>
   </si>
   <si>
-    <t>Heavy  Snow Blowing Snow Mist</t>
-  </si>
-  <si>
-    <t>Light  Ice Pellet Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Pellet Showers</t>
-  </si>
-  <si>
-    <t>Light  Hail Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Hail Showers</t>
-  </si>
-  <si>
-    <t>Light  Small Hail Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Small Hail Showers</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorm</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorm</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Rain</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Snow</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Ice Pellets</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Ice Pellets</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms with Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms with Hail</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms with Small Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms with Small Hail</t>
-  </si>
-  <si>
-    <t>Light  Freezing Drizzle</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Drizzle</t>
-  </si>
-  <si>
-    <t>Light  Freezing Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Rain</t>
-  </si>
-  <si>
-    <t>Light  Freezing Fog</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Fog</t>
-  </si>
-  <si>
     <t>Removed arm warmers last part of ride</t>
   </si>
   <si>
@@ -598,6 +373,240 @@
   </si>
   <si>
     <t>Too warm</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Sand</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Snow</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Widespread Dust</t>
+  </si>
+  <si>
+    <t>Heavy Dust Whirls</t>
+  </si>
+  <si>
+    <t>Heavy Fog</t>
+  </si>
+  <si>
+    <t>Heavy Fog Patches</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Drizzle</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Fog</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Rain</t>
+  </si>
+  <si>
+    <t>Heavy Hail</t>
+  </si>
+  <si>
+    <t>Heavy Hail Showers</t>
+  </si>
+  <si>
+    <t>Heavy Haze</t>
+  </si>
+  <si>
+    <t>Heavy Ice Crystals</t>
+  </si>
+  <si>
+    <t>Heavy Ice Pellet Showers</t>
+  </si>
+  <si>
+    <t>Heavy Ice Pellets</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Sand</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Snow</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Widespread Dust</t>
+  </si>
+  <si>
+    <t>Heavy Mist</t>
+  </si>
+  <si>
+    <t>Heavy Rain</t>
+  </si>
+  <si>
+    <t>Heavy Rain Mist</t>
+  </si>
+  <si>
+    <t>Heavy Rain Showers</t>
+  </si>
+  <si>
+    <t>Heavy Sand</t>
+  </si>
+  <si>
+    <t>Heavy Sandstorm</t>
+  </si>
+  <si>
+    <t>Heavy Small Hail Showers</t>
+  </si>
+  <si>
+    <t>Heavy Smoke</t>
+  </si>
+  <si>
+    <t>Heavy Snow</t>
+  </si>
+  <si>
+    <t>Heavy Snow Blowing Snow Mist</t>
+  </si>
+  <si>
+    <t>Heavy Snow Grains</t>
+  </si>
+  <si>
+    <t>Heavy Snow Showers</t>
+  </si>
+  <si>
+    <t>Heavy Spray</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorm</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Ice Pellets</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Rain</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Snow</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms with Hail</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms with Small Hail</t>
+  </si>
+  <si>
+    <t>Heavy Volcanic Ash</t>
+  </si>
+  <si>
+    <t>Heavy Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Blowing Sand</t>
+  </si>
+  <si>
+    <t>Light Blowing Snow</t>
+  </si>
+  <si>
+    <t>Light Blowing Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Dust Whirls</t>
+  </si>
+  <si>
+    <t>Light Fog</t>
+  </si>
+  <si>
+    <t>Light Fog Patches</t>
+  </si>
+  <si>
+    <t>Light Freezing Drizzle</t>
+  </si>
+  <si>
+    <t>Light Freezing Fog</t>
+  </si>
+  <si>
+    <t>Light Freezing Rain</t>
+  </si>
+  <si>
+    <t>Light Hail</t>
+  </si>
+  <si>
+    <t>Light Hail Showers</t>
+  </si>
+  <si>
+    <t>Light Haze</t>
+  </si>
+  <si>
+    <t>Light Ice Crystals</t>
+  </si>
+  <si>
+    <t>Light Ice Pellet Showers</t>
+  </si>
+  <si>
+    <t>Light Ice Pellets</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Sand</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Snow</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Mist</t>
+  </si>
+  <si>
+    <t>Light Rain</t>
+  </si>
+  <si>
+    <t>Light Rain Mist</t>
+  </si>
+  <si>
+    <t>Light Rain Showers</t>
+  </si>
+  <si>
+    <t>Light Sand</t>
+  </si>
+  <si>
+    <t>Light Sandstorm</t>
+  </si>
+  <si>
+    <t>Light Small Hail Showers</t>
+  </si>
+  <si>
+    <t>Light Smoke</t>
+  </si>
+  <si>
+    <t>Light Snow</t>
+  </si>
+  <si>
+    <t>Light Snow Blowing Snow Mist</t>
+  </si>
+  <si>
+    <t>Light Snow Grains</t>
+  </si>
+  <si>
+    <t>Light Snow Showers</t>
+  </si>
+  <si>
+    <t>Light Spray</t>
+  </si>
+  <si>
+    <t>Light Thunderstorm</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Ice Pellets</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Rain</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Snow</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms with Hail</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms with Small Hail</t>
+  </si>
+  <si>
+    <t>Light Volcanic Ash</t>
+  </si>
+  <si>
+    <t>Light Widespread Dust</t>
   </si>
 </sst>
 </file>
@@ -970,8 +979,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y36" totalsRowShown="0">
-  <autoFilter ref="A1:Y36" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y39" totalsRowShown="0">
+  <autoFilter ref="A1:Y39" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y26">
     <sortCondition ref="B1:B26"/>
   </sortState>
@@ -1405,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC4919-1670-4AFD-91C3-CDFEF0B7A9A5}">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="H36" sqref="H36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1428,7 @@
     <col min="10" max="10" width="9.77734375" customWidth="1"/>
     <col min="12" max="12" width="10.21875" customWidth="1"/>
     <col min="13" max="15" width="10.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.88671875" customWidth="1"/>
     <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -1445,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -1472,13 +1481,13 @@
         <v>26</v>
       </c>
       <c r="P1" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>159</v>
+        <v>84</v>
       </c>
       <c r="R1" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -1490,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="V1" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="W1" t="s">
         <v>24</v>
@@ -1499,7 +1508,7 @@
         <v>50</v>
       </c>
       <c r="Y1" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1550,28 +1559,28 @@
         <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s">
         <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U2" t="s">
         <v>29</v>
       </c>
       <c r="V2" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W2" t="s">
         <v>29</v>
       </c>
       <c r="X2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y2" t="s">
         <v>29</v>
@@ -1625,28 +1634,28 @@
         <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R3" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
       </c>
       <c r="T3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U3" t="s">
         <v>29</v>
       </c>
       <c r="V3" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W3" t="s">
         <v>38</v>
       </c>
       <c r="X3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y3" t="s">
         <v>29</v>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>19</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1707,16 +1716,16 @@
         <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S4" t="s">
         <v>29</v>
       </c>
       <c r="T4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U4" t="s">
         <v>29</v>
@@ -1728,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="X4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y4" t="s">
         <v>29</v>
@@ -1738,7 +1747,7 @@
       </c>
       <c r="AB4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>7</v>
+        <v>12</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1789,16 +1798,16 @@
         <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R5" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S5" t="s">
         <v>29</v>
       </c>
       <c r="T5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U5" t="s">
         <v>29</v>
@@ -1810,7 +1819,7 @@
         <v>29</v>
       </c>
       <c r="X5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y5" t="s">
         <v>29</v>
@@ -1820,7 +1829,7 @@
       </c>
       <c r="AB5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>52</v>
+        <v>65</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1873,16 +1882,16 @@
         <v>29</v>
       </c>
       <c r="Q6" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R6" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S6" t="s">
         <v>29</v>
       </c>
       <c r="T6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U6" t="s">
         <v>30</v>
@@ -1894,7 +1903,7 @@
         <v>29</v>
       </c>
       <c r="X6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y6" t="s">
         <v>29</v>
@@ -1948,28 +1957,28 @@
         <v>29</v>
       </c>
       <c r="Q7" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R7" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S7" t="s">
         <v>29</v>
       </c>
       <c r="T7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U7" t="s">
         <v>29</v>
       </c>
       <c r="V7" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W7" t="s">
         <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y7" t="s">
         <v>29</v>
@@ -2023,10 +2032,10 @@
         <v>30</v>
       </c>
       <c r="Q8" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R8" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S8" t="s">
         <v>29</v>
@@ -2038,13 +2047,13 @@
         <v>30</v>
       </c>
       <c r="V8" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W8" t="s">
         <v>38</v>
       </c>
       <c r="X8" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y8" t="s">
         <v>29</v>
@@ -2098,16 +2107,16 @@
         <v>29</v>
       </c>
       <c r="Q9" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S9" t="s">
         <v>29</v>
       </c>
       <c r="T9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U9" t="s">
         <v>29</v>
@@ -2119,7 +2128,7 @@
         <v>29</v>
       </c>
       <c r="X9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y9" t="s">
         <v>29</v>
@@ -2173,28 +2182,28 @@
         <v>30</v>
       </c>
       <c r="Q10" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R10" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S10" t="s">
         <v>29</v>
       </c>
       <c r="T10" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U10" t="s">
         <v>30</v>
       </c>
       <c r="V10" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W10" t="s">
         <v>29</v>
       </c>
       <c r="X10" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y10" t="s">
         <v>29</v>
@@ -2248,28 +2257,28 @@
         <v>30</v>
       </c>
       <c r="Q11" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R11" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S11" t="s">
         <v>29</v>
       </c>
       <c r="T11" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U11" t="s">
         <v>30</v>
       </c>
       <c r="V11" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W11" t="s">
         <v>38</v>
       </c>
       <c r="X11" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y11" t="s">
         <v>29</v>
@@ -2323,28 +2332,28 @@
         <v>29</v>
       </c>
       <c r="Q12" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R12" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S12" t="s">
         <v>30</v>
       </c>
       <c r="T12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U12" t="s">
         <v>30</v>
       </c>
       <c r="V12" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W12" t="s">
         <v>38</v>
       </c>
       <c r="X12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y12" t="s">
         <v>29</v>
@@ -2370,7 +2379,7 @@
         <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>30</v>
@@ -2400,10 +2409,10 @@
         <v>30</v>
       </c>
       <c r="Q13" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R13" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S13" t="s">
         <v>29</v>
@@ -2415,13 +2424,13 @@
         <v>30</v>
       </c>
       <c r="V13" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W13" t="s">
         <v>38</v>
       </c>
       <c r="X13" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y13" t="s">
         <v>29</v>
@@ -2447,7 +2456,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>30</v>
@@ -2475,28 +2484,28 @@
         <v>30</v>
       </c>
       <c r="Q14" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R14" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S14" t="s">
         <v>29</v>
       </c>
       <c r="T14" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U14" t="s">
         <v>30</v>
       </c>
       <c r="V14" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W14" t="s">
         <v>38</v>
       </c>
       <c r="X14" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y14" t="s">
         <v>29</v>
@@ -2550,28 +2559,28 @@
         <v>30</v>
       </c>
       <c r="Q15" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R15" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S15" t="s">
         <v>29</v>
       </c>
       <c r="T15" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U15" t="s">
         <v>30</v>
       </c>
       <c r="V15" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W15" t="s">
         <v>38</v>
       </c>
       <c r="X15" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y15" t="s">
         <v>29</v>
@@ -2625,28 +2634,28 @@
         <v>29</v>
       </c>
       <c r="Q16" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S16" t="s">
         <v>29</v>
       </c>
       <c r="T16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U16" t="s">
         <v>29</v>
       </c>
       <c r="V16" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W16" t="s">
         <v>38</v>
       </c>
       <c r="X16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y16" t="s">
         <v>29</v>
@@ -2696,22 +2705,22 @@
         <v>27</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="P17" t="s">
         <v>29</v>
       </c>
       <c r="Q17" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S17" t="s">
         <v>30</v>
       </c>
       <c r="T17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U17" t="s">
         <v>29</v>
@@ -2723,7 +2732,7 @@
         <v>29</v>
       </c>
       <c r="X17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y17" t="s">
         <v>29</v>
@@ -2758,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5">
         <v>35</v>
@@ -2775,10 +2784,10 @@
         <v>30</v>
       </c>
       <c r="Q18" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R18" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S18" t="s">
         <v>29</v>
@@ -2790,13 +2799,13 @@
         <v>30</v>
       </c>
       <c r="V18" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W18" t="s">
         <v>38</v>
       </c>
       <c r="X18" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y18" t="s">
         <v>30</v>
@@ -2831,7 +2840,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K19" s="5">
         <v>45</v>
@@ -2850,16 +2859,16 @@
         <v>29</v>
       </c>
       <c r="Q19" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R19" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S19" t="s">
         <v>29</v>
       </c>
       <c r="T19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U19" t="s">
         <v>29</v>
@@ -2871,7 +2880,7 @@
         <v>38</v>
       </c>
       <c r="X19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y19" t="s">
         <v>29</v>
@@ -2921,34 +2930,34 @@
         <v>49</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
       </c>
       <c r="Q20" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R20" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S20" t="s">
         <v>29</v>
       </c>
       <c r="T20" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U20" t="s">
         <v>30</v>
       </c>
       <c r="V20" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W20" t="s">
         <v>29</v>
       </c>
       <c r="X20" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y20" t="s">
         <v>29</v>
@@ -3002,16 +3011,16 @@
         <v>29</v>
       </c>
       <c r="Q21" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R21" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S21" t="s">
         <v>29</v>
       </c>
       <c r="T21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U21" t="s">
         <v>29</v>
@@ -3023,7 +3032,7 @@
         <v>38</v>
       </c>
       <c r="X21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y21" t="s">
         <v>29</v>
@@ -3058,7 +3067,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="K22" s="5">
         <v>55</v>
@@ -3077,16 +3086,16 @@
         <v>29</v>
       </c>
       <c r="Q22" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R22" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S22" t="s">
         <v>29</v>
       </c>
       <c r="T22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U22" t="s">
         <v>29</v>
@@ -3098,7 +3107,7 @@
         <v>29</v>
       </c>
       <c r="X22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y22" t="s">
         <v>29</v>
@@ -3150,16 +3159,16 @@
         <v>29</v>
       </c>
       <c r="Q23" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R23" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S23" t="s">
         <v>29</v>
       </c>
       <c r="T23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U23" t="s">
         <v>29</v>
@@ -3171,7 +3180,7 @@
         <v>29</v>
       </c>
       <c r="X23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y23" t="s">
         <v>29</v>
@@ -3206,7 +3215,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K24" s="5">
         <v>48</v>
@@ -3223,28 +3232,28 @@
         <v>29</v>
       </c>
       <c r="Q24" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S24" t="s">
         <v>29</v>
       </c>
       <c r="T24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U24" t="s">
         <v>29</v>
       </c>
       <c r="V24" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W24" t="s">
         <v>29</v>
       </c>
       <c r="X24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y24" t="s">
         <v>29</v>
@@ -3279,7 +3288,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K25" s="5">
         <v>30</v>
@@ -3296,28 +3305,28 @@
         <v>30</v>
       </c>
       <c r="Q25" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R25" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S25" t="s">
         <v>29</v>
       </c>
       <c r="T25" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U25" t="s">
         <v>30</v>
       </c>
       <c r="V25" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W25" t="s">
         <v>29</v>
       </c>
       <c r="X25" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y25" t="s">
         <v>29</v>
@@ -3352,7 +3361,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="K26" s="5">
         <v>55</v>
@@ -3364,35 +3373,35 @@
         <v>0.88</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s">
         <v>29</v>
       </c>
       <c r="Q26" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S26" t="s">
         <v>29</v>
       </c>
       <c r="T26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U26" t="s">
         <v>30</v>
       </c>
       <c r="V26" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W26" t="s">
         <v>29</v>
       </c>
       <c r="X26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y26" t="s">
         <v>29</v>
@@ -3427,7 +3436,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="K27" s="5">
         <v>43</v>
@@ -3439,17 +3448,17 @@
         <v>0.61</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s">
         <v>29</v>
       </c>
       <c r="Q27" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R27" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S27" t="s">
         <v>29</v>
@@ -3461,13 +3470,13 @@
         <v>29</v>
       </c>
       <c r="V27" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W27" t="s">
         <v>29</v>
       </c>
       <c r="X27" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y27" t="s">
         <v>29</v>
@@ -3484,7 +3493,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="E28" s="5">
         <v>30.5</v>
@@ -3502,7 +3511,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K28" s="5">
         <v>44</v>
@@ -3521,10 +3530,10 @@
         <v>30</v>
       </c>
       <c r="Q28" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R28" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S28" t="s">
         <v>30</v>
@@ -3536,13 +3545,13 @@
         <v>30</v>
       </c>
       <c r="V28" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W28" t="s">
         <v>30</v>
       </c>
       <c r="X28" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y28" t="s">
         <v>29</v>
@@ -3577,7 +3586,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="K29" s="5">
         <v>39</v>
@@ -3589,35 +3598,35 @@
         <v>0.65</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s">
         <v>29</v>
       </c>
       <c r="Q29" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R29" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S29" t="s">
         <v>29</v>
       </c>
       <c r="T29" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U29" t="s">
         <v>29</v>
       </c>
       <c r="V29" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W29" t="s">
         <v>29</v>
       </c>
       <c r="X29" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y29" t="s">
         <v>29</v>
@@ -3669,28 +3678,28 @@
         <v>29</v>
       </c>
       <c r="Q30" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R30" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S30" t="s">
         <v>29</v>
       </c>
       <c r="T30" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U30" t="s">
         <v>29</v>
       </c>
       <c r="V30" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W30" t="s">
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y30" t="s">
         <v>29</v>
@@ -3725,7 +3734,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -3742,28 +3751,28 @@
         <v>30</v>
       </c>
       <c r="Q31" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R31" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S31" t="s">
         <v>29</v>
       </c>
       <c r="T31" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U31" t="s">
         <v>30</v>
       </c>
       <c r="V31" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W31" t="s">
         <v>38</v>
       </c>
       <c r="X31" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y31" t="s">
         <v>29</v>
@@ -3798,7 +3807,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K32" s="5">
         <v>36</v>
@@ -3815,28 +3824,28 @@
         <v>29</v>
       </c>
       <c r="Q32" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S32" t="s">
         <v>29</v>
       </c>
       <c r="T32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U32" t="s">
         <v>30</v>
       </c>
       <c r="V32" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W32" t="s">
         <v>29</v>
       </c>
       <c r="X32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y32" t="s">
         <v>29</v>
@@ -3888,28 +3897,28 @@
         <v>30</v>
       </c>
       <c r="Q33" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="R33" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S33" t="s">
         <v>29</v>
       </c>
       <c r="T33" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="U33" t="s">
         <v>30</v>
       </c>
       <c r="V33" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W33" t="s">
         <v>30</v>
       </c>
       <c r="X33" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y33" t="s">
         <v>29</v>
@@ -3961,16 +3970,16 @@
         <v>29</v>
       </c>
       <c r="Q34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="R34" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S34" t="s">
         <v>29</v>
       </c>
       <c r="T34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U34" t="s">
         <v>29</v>
@@ -3982,7 +3991,7 @@
         <v>29</v>
       </c>
       <c r="X34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y34" t="s">
         <v>29</v>
@@ -4017,7 +4026,7 @@
         <v>9</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="K35" s="5">
         <v>25</v>
@@ -4029,62 +4038,285 @@
         <v>0.8</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>183</v>
+        <v>108</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s">
         <v>30</v>
       </c>
       <c r="Q35" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R35" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S35" t="s">
         <v>29</v>
       </c>
       <c r="T35" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U35" t="s">
         <v>30</v>
       </c>
       <c r="V35" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W35" t="s">
         <v>38</v>
       </c>
       <c r="X35" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="7"/>
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1">
+        <v>43830</v>
+      </c>
+      <c r="C36" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2</v>
+      </c>
+      <c r="F36" s="6">
+        <v>22</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="5">
+        <v>9</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36" s="5">
+        <v>45</v>
+      </c>
+      <c r="L36" s="5">
+        <v>41</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0.86</v>
+      </c>
       <c r="N36" s="7"/>
       <c r="O36" s="2"/>
+      <c r="P36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>88</v>
+      </c>
+      <c r="R36" t="s">
+        <v>82</v>
+      </c>
+      <c r="S36" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" t="s">
+        <v>82</v>
+      </c>
+      <c r="U36" t="s">
+        <v>29</v>
+      </c>
+      <c r="V36" t="s">
+        <v>20</v>
+      </c>
+      <c r="W36" t="s">
+        <v>29</v>
+      </c>
+      <c r="X36" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43466</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="F37" s="6">
+        <v>60</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="5">
+        <v>9</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="5">
+        <v>28</v>
+      </c>
+      <c r="L37" s="5">
+        <v>20</v>
+      </c>
+      <c r="M37" s="7">
+        <v>1</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" t="s">
+        <v>88</v>
+      </c>
+      <c r="S37" t="s">
+        <v>29</v>
+      </c>
+      <c r="T37" t="s">
+        <v>103</v>
+      </c>
+      <c r="U37" t="s">
+        <v>30</v>
+      </c>
+      <c r="V37" t="s">
+        <v>93</v>
+      </c>
+      <c r="W37" t="s">
+        <v>38</v>
+      </c>
+      <c r="X37" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="F38" s="6">
+        <v>40</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="5">
+        <v>8</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K38" s="5">
+        <v>37</v>
+      </c>
+      <c r="L38" s="5">
+        <v>32</v>
+      </c>
+      <c r="M38" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>89</v>
+      </c>
+      <c r="R38" t="s">
+        <v>87</v>
+      </c>
+      <c r="S38" t="s">
+        <v>29</v>
+      </c>
+      <c r="T38" t="s">
+        <v>82</v>
+      </c>
+      <c r="U38" t="s">
+        <v>30</v>
+      </c>
+      <c r="V38" t="s">
+        <v>94</v>
+      </c>
+      <c r="W38" t="s">
+        <v>29</v>
+      </c>
+      <c r="X38" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="B39" s="1"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="6"/>
+      <c r="H39" s="5"/>
+      <c r="I39" s="5"/>
+      <c r="J39" s="5"/>
+      <c r="K39" s="5"/>
+      <c r="L39" s="5"/>
+      <c r="M39" s="7"/>
+      <c r="N39" s="7"/>
+      <c r="O39" s="2"/>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G36" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G39" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
       <formula1>Conditions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T36" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T39" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
       <formula1>JacketOption</formula1>
     </dataValidation>
   </dataValidations>
@@ -4100,25 +4332,25 @@
           <x14:formula1>
             <xm:f>ValidValues!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P36 S2:S36 U2:U36 W2:W36 Y2:Y36</xm:sqref>
+          <xm:sqref>P2:P39 S2:S39 U2:U39 W2:W39 Y2:Y39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BFEBF07-64B2-450B-BC13-447B52D5D711}">
           <x14:formula1>
             <xm:f>ValidValues!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:R36</xm:sqref>
+          <xm:sqref>Q2:R39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E09EE0F-16F0-4536-B318-2F013ED3F6AB}">
           <x14:formula1>
             <xm:f>ValidValues!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V36</xm:sqref>
+          <xm:sqref>V2:V39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1617D946-B125-4BE6-B340-3AE6EE661815}">
           <x14:formula1>
             <xm:f>ValidValues!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X36</xm:sqref>
+          <xm:sqref>X2:X39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4165,7 +4397,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -4231,7 +4463,7 @@
         <v>50</v>
       </c>
       <c r="AC1" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -4306,7 +4538,7 @@
         <v>30</v>
       </c>
       <c r="Y2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z2" t="s">
         <v>30</v>
@@ -4393,7 +4625,7 @@
         <v>30</v>
       </c>
       <c r="Y3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z3" t="s">
         <v>30</v>
@@ -4412,7 +4644,7 @@
       </c>
       <c r="AF3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>77</v>
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -4487,7 +4719,7 @@
         <v>30</v>
       </c>
       <c r="Y4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z4" t="s">
         <v>29</v>
@@ -4506,7 +4738,7 @@
       </c>
       <c r="AF4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -4581,7 +4813,7 @@
         <v>30</v>
       </c>
       <c r="Y5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z5" t="s">
         <v>29</v>
@@ -4600,7 +4832,7 @@
       </c>
       <c r="AF5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -4677,7 +4909,7 @@
         <v>30</v>
       </c>
       <c r="Y6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z6" t="s">
         <v>29</v>
@@ -4764,7 +4996,7 @@
         <v>30</v>
       </c>
       <c r="Y7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z7" t="s">
         <v>30</v>
@@ -4851,7 +5083,7 @@
         <v>29</v>
       </c>
       <c r="Y8" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z8" t="s">
         <v>29</v>
@@ -4938,7 +5170,7 @@
         <v>30</v>
       </c>
       <c r="Y9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z9" t="s">
         <v>29</v>
@@ -5025,7 +5257,7 @@
         <v>29</v>
       </c>
       <c r="Y10" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z10" t="s">
         <v>29</v>
@@ -5112,7 +5344,7 @@
         <v>29</v>
       </c>
       <c r="Y11" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z11" t="s">
         <v>29</v>
@@ -5199,7 +5431,7 @@
         <v>30</v>
       </c>
       <c r="Y12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z12" t="s">
         <v>30</v>
@@ -5234,7 +5466,7 @@
         <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>30</v>
@@ -5288,7 +5520,7 @@
         <v>29</v>
       </c>
       <c r="Y13" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z13" t="s">
         <v>29</v>
@@ -5323,7 +5555,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>30</v>
@@ -5375,7 +5607,7 @@
         <v>29</v>
       </c>
       <c r="Y14" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z14" t="s">
         <v>29</v>
@@ -5462,7 +5694,7 @@
         <v>29</v>
       </c>
       <c r="Y15" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z15" t="s">
         <v>29</v>
@@ -5549,7 +5781,7 @@
         <v>30</v>
       </c>
       <c r="Y16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z16" t="s">
         <v>30</v>
@@ -5608,7 +5840,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="P17" t="s">
         <v>29</v>
@@ -5638,7 +5870,7 @@
         <v>30</v>
       </c>
       <c r="Y17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z17" t="s">
         <v>29</v>
@@ -5682,7 +5914,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5">
         <v>35</v>
@@ -5723,7 +5955,7 @@
         <v>29</v>
       </c>
       <c r="Y18" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z18" t="s">
         <v>29</v>
@@ -5767,7 +5999,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K19" s="5">
         <v>45</v>
@@ -5810,7 +6042,7 @@
         <v>30</v>
       </c>
       <c r="Y19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z19" t="s">
         <v>29</v>
@@ -5869,7 +6101,7 @@
         <v>49</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="P20" t="s">
         <v>29</v>
@@ -5899,7 +6131,7 @@
         <v>29</v>
       </c>
       <c r="Y20" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z20" t="s">
         <v>29</v>
@@ -5986,7 +6218,7 @@
         <v>30</v>
       </c>
       <c r="Y21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z21" t="s">
         <v>29</v>
@@ -6030,7 +6262,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="K22" s="5">
         <v>55</v>
@@ -6073,7 +6305,7 @@
         <v>30</v>
       </c>
       <c r="Y22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z22" t="s">
         <v>29</v>
@@ -6158,7 +6390,7 @@
         <v>30</v>
       </c>
       <c r="Y23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z23" t="s">
         <v>29</v>
@@ -6202,7 +6434,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K24" s="5">
         <v>48</v>
@@ -6243,7 +6475,7 @@
         <v>30</v>
       </c>
       <c r="Y24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z24" t="s">
         <v>30</v>
@@ -6287,7 +6519,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K25" s="5">
         <v>30</v>
@@ -6328,7 +6560,7 @@
         <v>29</v>
       </c>
       <c r="Y25" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z25" t="s">
         <v>29</v>
@@ -6372,7 +6604,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="K26" s="5">
         <v>55</v>
@@ -6384,7 +6616,7 @@
         <v>0.88</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s">
@@ -6415,7 +6647,7 @@
         <v>30</v>
       </c>
       <c r="Y26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z26" t="s">
         <v>30</v>
@@ -6459,7 +6691,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="K27" s="5">
         <v>43</v>
@@ -6471,7 +6703,7 @@
         <v>0.61</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s">
@@ -6502,7 +6734,7 @@
         <v>30</v>
       </c>
       <c r="Y27" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z27" t="s">
         <v>30</v>
@@ -6528,7 +6760,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="E28" s="5">
         <v>30.5</v>
@@ -6546,7 +6778,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K28" s="5">
         <v>44</v>
@@ -6589,7 +6821,7 @@
         <v>29</v>
       </c>
       <c r="Y28" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z28" t="s">
         <v>29</v>
@@ -6633,7 +6865,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="K29" s="5">
         <v>39</v>
@@ -6645,7 +6877,7 @@
         <v>0.65</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s">
@@ -6676,7 +6908,7 @@
         <v>29</v>
       </c>
       <c r="Y29" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z29" t="s">
         <v>29</v>
@@ -6761,7 +6993,7 @@
         <v>29</v>
       </c>
       <c r="Y30" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z30" t="s">
         <v>29</v>
@@ -6805,7 +7037,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -6846,7 +7078,7 @@
         <v>29</v>
       </c>
       <c r="Y31" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z31" t="s">
         <v>29</v>
@@ -6913,8 +7145,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF5CF31-5DCF-45F0-99A9-605CADC9A594}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6931,22 +7163,22 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="J1" t="s">
-        <v>175</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6957,19 +7189,19 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6980,19 +7212,19 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -7000,237 +7232,237 @@
         <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>177</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="H7" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>51</v>
@@ -7238,7 +7470,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>52</v>
@@ -7254,7 +7486,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>54</v>
@@ -7262,7 +7494,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>35</v>
@@ -7270,7 +7502,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>31</v>
@@ -7278,7 +7510,7 @@
     </row>
     <row r="47" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>55</v>
@@ -7286,7 +7518,7 @@
     </row>
     <row r="48" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>56</v>
@@ -7294,7 +7526,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>57</v>
@@ -7302,7 +7534,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>58</v>
@@ -7310,7 +7542,7 @@
     </row>
     <row r="51" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>59</v>
@@ -7318,7 +7550,7 @@
     </row>
     <row r="52" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>60</v>
@@ -7326,7 +7558,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>61</v>
@@ -7334,147 +7566,147 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
@@ -7579,7 +7811,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>32</v>
@@ -7648,7 +7880,7 @@
         <v>50</v>
       </c>
       <c r="AA1" s="10" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Separated out the Location into a new class.  Added comments for how to handle saving/reading the forecast and historical observations from a file.  Not a working version.
</commit_message>
<xml_diff>
--- a/what_to_wear_outdoors/data/What I wore running.xlsx
+++ b/what_to_wear_outdoors/data/What I wore running.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c10a0a3541b6f8b5/Fitness/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="28" documentId="104_{AECD96ED-7C4A-43C3-A65D-5FA5035B2AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{4560FAD1-0D85-4DD7-80A1-E79495EA9D66}"/>
+  <xr:revisionPtr revIDLastSave="132" documentId="104_{AECD96ED-7C4A-43C3-A65D-5FA5035B2AB1}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{97DC4FC9-4863-4659-83AA-08EFF59271A7}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="12936" windowHeight="3360" xr2:uid="{0E554CF6-5D67-46BF-86F7-11F8583F5090}"/>
   </bookViews>
@@ -46,7 +46,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1385" uniqueCount="184">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1448" uniqueCount="187">
   <si>
     <t>Run</t>
   </si>
@@ -240,240 +240,15 @@
     <t>Heavy Drizzel</t>
   </si>
   <si>
-    <t>Light  Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Rain</t>
-  </si>
-  <si>
     <t>Light  Snow</t>
   </si>
   <si>
-    <t>Heavy  Snow</t>
-  </si>
-  <si>
-    <t>Light  Snow Grains</t>
-  </si>
-  <si>
-    <t>Heavy  Snow Grains</t>
-  </si>
-  <si>
-    <t>Light  Ice Crystals</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Crystals</t>
-  </si>
-  <si>
-    <t>Light  Ice Pellets</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Pellets</t>
-  </si>
-  <si>
-    <t>Light  Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Hail</t>
-  </si>
-  <si>
     <t>Light  Mist</t>
   </si>
   <si>
-    <t>Heavy  Mist</t>
-  </si>
-  <si>
-    <t>Light  Fog</t>
-  </si>
-  <si>
-    <t>Heavy  Fog</t>
-  </si>
-  <si>
-    <t>Light  Fog Patches</t>
-  </si>
-  <si>
-    <t>Heavy  Fog Patches</t>
-  </si>
-  <si>
-    <t>Light  Smoke</t>
-  </si>
-  <si>
-    <t>Heavy  Smoke</t>
-  </si>
-  <si>
-    <t>Light  Volcanic Ash</t>
-  </si>
-  <si>
-    <t>Heavy  Volcanic Ash</t>
-  </si>
-  <si>
-    <t>Light  Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Sand</t>
-  </si>
-  <si>
-    <t>Light  Haze</t>
-  </si>
-  <si>
-    <t>Heavy  Haze</t>
-  </si>
-  <si>
-    <t>Light  Spray</t>
-  </si>
-  <si>
-    <t>Heavy  Spray</t>
-  </si>
-  <si>
-    <t>Light  Dust Whirls</t>
-  </si>
-  <si>
-    <t>Heavy  Dust Whirls</t>
-  </si>
-  <si>
-    <t>Light  Sandstorm</t>
-  </si>
-  <si>
-    <t>Heavy  Sandstorm</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Snow</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Low Drifting Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Low Drifting Sand</t>
-  </si>
-  <si>
-    <t>Light  Blowing Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Snow</t>
-  </si>
-  <si>
-    <t>Light  Blowing Widespread Dust</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Widespread Dust</t>
-  </si>
-  <si>
-    <t>Light  Blowing Sand</t>
-  </si>
-  <si>
-    <t>Heavy  Blowing Sand</t>
-  </si>
-  <si>
-    <t>Light  Rain Mist</t>
-  </si>
-  <si>
-    <t>Heavy  Rain Mist</t>
-  </si>
-  <si>
-    <t>Light  Rain Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Rain Showers</t>
-  </si>
-  <si>
-    <t>Light  Snow Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Snow Showers</t>
-  </si>
-  <si>
     <t>Light  Snow Blowing Snow Mist</t>
   </si>
   <si>
-    <t>Heavy  Snow Blowing Snow Mist</t>
-  </si>
-  <si>
-    <t>Light  Ice Pellet Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Ice Pellet Showers</t>
-  </si>
-  <si>
-    <t>Light  Hail Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Hail Showers</t>
-  </si>
-  <si>
-    <t>Light  Small Hail Showers</t>
-  </si>
-  <si>
-    <t>Heavy  Small Hail Showers</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorm</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorm</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Rain</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Snow</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Snow</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms and Ice Pellets</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms and Ice Pellets</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms with Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms with Hail</t>
-  </si>
-  <si>
-    <t>Light  Thunderstorms with Small Hail</t>
-  </si>
-  <si>
-    <t>Heavy  Thunderstorms with Small Hail</t>
-  </si>
-  <si>
-    <t>Light  Freezing Drizzle</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Drizzle</t>
-  </si>
-  <si>
-    <t>Light  Freezing Rain</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Rain</t>
-  </si>
-  <si>
-    <t>Light  Freezing Fog</t>
-  </si>
-  <si>
-    <t>Heavy  Freezing Fog</t>
-  </si>
-  <si>
     <t>Removed arm warmers last part of ride</t>
   </si>
   <si>
@@ -598,6 +373,240 @@
   </si>
   <si>
     <t>Too warm</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Sand</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Snow</t>
+  </si>
+  <si>
+    <t>Heavy Blowing Widespread Dust</t>
+  </si>
+  <si>
+    <t>Heavy Dust Whirls</t>
+  </si>
+  <si>
+    <t>Heavy Fog</t>
+  </si>
+  <si>
+    <t>Heavy Fog Patches</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Drizzle</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Fog</t>
+  </si>
+  <si>
+    <t>Heavy Freezing Rain</t>
+  </si>
+  <si>
+    <t>Heavy Hail</t>
+  </si>
+  <si>
+    <t>Heavy Hail Showers</t>
+  </si>
+  <si>
+    <t>Heavy Haze</t>
+  </si>
+  <si>
+    <t>Heavy Ice Crystals</t>
+  </si>
+  <si>
+    <t>Heavy Ice Pellet Showers</t>
+  </si>
+  <si>
+    <t>Heavy Ice Pellets</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Sand</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Snow</t>
+  </si>
+  <si>
+    <t>Heavy Low Drifting Widespread Dust</t>
+  </si>
+  <si>
+    <t>Heavy Mist</t>
+  </si>
+  <si>
+    <t>Heavy Rain</t>
+  </si>
+  <si>
+    <t>Heavy Rain Mist</t>
+  </si>
+  <si>
+    <t>Heavy Rain Showers</t>
+  </si>
+  <si>
+    <t>Heavy Sand</t>
+  </si>
+  <si>
+    <t>Heavy Sandstorm</t>
+  </si>
+  <si>
+    <t>Heavy Small Hail Showers</t>
+  </si>
+  <si>
+    <t>Heavy Smoke</t>
+  </si>
+  <si>
+    <t>Heavy Snow</t>
+  </si>
+  <si>
+    <t>Heavy Snow Blowing Snow Mist</t>
+  </si>
+  <si>
+    <t>Heavy Snow Grains</t>
+  </si>
+  <si>
+    <t>Heavy Snow Showers</t>
+  </si>
+  <si>
+    <t>Heavy Spray</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorm</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Ice Pellets</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Rain</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms and Snow</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms with Hail</t>
+  </si>
+  <si>
+    <t>Heavy Thunderstorms with Small Hail</t>
+  </si>
+  <si>
+    <t>Heavy Volcanic Ash</t>
+  </si>
+  <si>
+    <t>Heavy Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Blowing Sand</t>
+  </si>
+  <si>
+    <t>Light Blowing Snow</t>
+  </si>
+  <si>
+    <t>Light Blowing Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Dust Whirls</t>
+  </si>
+  <si>
+    <t>Light Fog</t>
+  </si>
+  <si>
+    <t>Light Fog Patches</t>
+  </si>
+  <si>
+    <t>Light Freezing Drizzle</t>
+  </si>
+  <si>
+    <t>Light Freezing Fog</t>
+  </si>
+  <si>
+    <t>Light Freezing Rain</t>
+  </si>
+  <si>
+    <t>Light Hail</t>
+  </si>
+  <si>
+    <t>Light Hail Showers</t>
+  </si>
+  <si>
+    <t>Light Haze</t>
+  </si>
+  <si>
+    <t>Light Ice Crystals</t>
+  </si>
+  <si>
+    <t>Light Ice Pellet Showers</t>
+  </si>
+  <si>
+    <t>Light Ice Pellets</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Sand</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Snow</t>
+  </si>
+  <si>
+    <t>Light Low Drifting Widespread Dust</t>
+  </si>
+  <si>
+    <t>Light Mist</t>
+  </si>
+  <si>
+    <t>Light Rain</t>
+  </si>
+  <si>
+    <t>Light Rain Mist</t>
+  </si>
+  <si>
+    <t>Light Rain Showers</t>
+  </si>
+  <si>
+    <t>Light Sand</t>
+  </si>
+  <si>
+    <t>Light Sandstorm</t>
+  </si>
+  <si>
+    <t>Light Small Hail Showers</t>
+  </si>
+  <si>
+    <t>Light Smoke</t>
+  </si>
+  <si>
+    <t>Light Snow</t>
+  </si>
+  <si>
+    <t>Light Snow Blowing Snow Mist</t>
+  </si>
+  <si>
+    <t>Light Snow Grains</t>
+  </si>
+  <si>
+    <t>Light Snow Showers</t>
+  </si>
+  <si>
+    <t>Light Spray</t>
+  </si>
+  <si>
+    <t>Light Thunderstorm</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Ice Pellets</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Rain</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms and Snow</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms with Hail</t>
+  </si>
+  <si>
+    <t>Light Thunderstorms with Small Hail</t>
+  </si>
+  <si>
+    <t>Light Volcanic Ash</t>
+  </si>
+  <si>
+    <t>Light Widespread Dust</t>
   </si>
 </sst>
 </file>
@@ -970,8 +979,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y36" totalsRowShown="0">
-  <autoFilter ref="A1:Y36" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{A450D7A5-304C-40FA-9B79-497989BF85D3}" name="Table16" displayName="Table16" ref="A1:Y39" totalsRowShown="0">
+  <autoFilter ref="A1:Y39" xr:uid="{3CAC4880-F62B-4E20-9BE8-8E7020B55855}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y26">
     <sortCondition ref="B1:B26"/>
   </sortState>
@@ -1405,10 +1414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{91BC4919-1670-4AFD-91C3-CDFEF0B7A9A5}">
-  <dimension ref="A1:AB36"/>
+  <dimension ref="A1:AB39"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="H40" sqref="H40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1419,7 +1428,7 @@
     <col min="10" max="10" width="9.77734375" customWidth="1"/>
     <col min="12" max="12" width="10.21875" customWidth="1"/>
     <col min="13" max="15" width="10.109375" customWidth="1"/>
-    <col min="16" max="16" width="11.21875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.109375" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="14.88671875" customWidth="1"/>
     <col min="18" max="18" width="11.5546875" bestFit="1" customWidth="1"/>
     <col min="22" max="22" width="15.44140625" bestFit="1" customWidth="1"/>
@@ -1445,7 +1454,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -1472,13 +1481,13 @@
         <v>26</v>
       </c>
       <c r="P1" t="s">
-        <v>174</v>
+        <v>99</v>
       </c>
       <c r="Q1" t="s">
-        <v>159</v>
+        <v>84</v>
       </c>
       <c r="R1" t="s">
-        <v>167</v>
+        <v>92</v>
       </c>
       <c r="S1" t="s">
         <v>17</v>
@@ -1490,7 +1499,7 @@
         <v>19</v>
       </c>
       <c r="V1" t="s">
-        <v>172</v>
+        <v>97</v>
       </c>
       <c r="W1" t="s">
         <v>24</v>
@@ -1499,7 +1508,7 @@
         <v>50</v>
       </c>
       <c r="Y1" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:28" x14ac:dyDescent="0.3">
@@ -1550,28 +1559,28 @@
         <v>29</v>
       </c>
       <c r="Q2" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S2" t="s">
         <v>29</v>
       </c>
       <c r="T2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U2" t="s">
         <v>29</v>
       </c>
       <c r="V2" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W2" t="s">
         <v>29</v>
       </c>
       <c r="X2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y2" t="s">
         <v>29</v>
@@ -1625,28 +1634,28 @@
         <v>29</v>
       </c>
       <c r="Q3" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R3" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S3" t="s">
         <v>29</v>
       </c>
       <c r="T3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U3" t="s">
         <v>29</v>
       </c>
       <c r="V3" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W3" t="s">
         <v>38</v>
       </c>
       <c r="X3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y3" t="s">
         <v>29</v>
@@ -1656,7 +1665,7 @@
       </c>
       <c r="AB3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>19</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.3">
@@ -1707,16 +1716,16 @@
         <v>29</v>
       </c>
       <c r="Q4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S4" t="s">
         <v>29</v>
       </c>
       <c r="T4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U4" t="s">
         <v>29</v>
@@ -1728,7 +1737,7 @@
         <v>29</v>
       </c>
       <c r="X4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y4" t="s">
         <v>29</v>
@@ -1738,7 +1747,7 @@
       </c>
       <c r="AB4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.3">
@@ -1789,16 +1798,16 @@
         <v>29</v>
       </c>
       <c r="Q5" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R5" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S5" t="s">
         <v>29</v>
       </c>
       <c r="T5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U5" t="s">
         <v>29</v>
@@ -1810,7 +1819,7 @@
         <v>29</v>
       </c>
       <c r="X5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y5" t="s">
         <v>29</v>
@@ -1820,7 +1829,7 @@
       </c>
       <c r="AB5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.3">
@@ -1873,16 +1882,16 @@
         <v>29</v>
       </c>
       <c r="Q6" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R6" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S6" t="s">
         <v>29</v>
       </c>
       <c r="T6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U6" t="s">
         <v>30</v>
@@ -1894,7 +1903,7 @@
         <v>29</v>
       </c>
       <c r="X6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y6" t="s">
         <v>29</v>
@@ -1948,28 +1957,28 @@
         <v>29</v>
       </c>
       <c r="Q7" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R7" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S7" t="s">
         <v>29</v>
       </c>
       <c r="T7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U7" t="s">
         <v>29</v>
       </c>
       <c r="V7" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W7" t="s">
         <v>38</v>
       </c>
       <c r="X7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y7" t="s">
         <v>29</v>
@@ -2023,10 +2032,10 @@
         <v>30</v>
       </c>
       <c r="Q8" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R8" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S8" t="s">
         <v>29</v>
@@ -2038,13 +2047,13 @@
         <v>30</v>
       </c>
       <c r="V8" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W8" t="s">
         <v>38</v>
       </c>
       <c r="X8" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y8" t="s">
         <v>29</v>
@@ -2098,16 +2107,16 @@
         <v>29</v>
       </c>
       <c r="Q9" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S9" t="s">
         <v>29</v>
       </c>
       <c r="T9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U9" t="s">
         <v>29</v>
@@ -2119,7 +2128,7 @@
         <v>29</v>
       </c>
       <c r="X9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y9" t="s">
         <v>29</v>
@@ -2173,28 +2182,28 @@
         <v>30</v>
       </c>
       <c r="Q10" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R10" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S10" t="s">
         <v>29</v>
       </c>
       <c r="T10" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U10" t="s">
         <v>30</v>
       </c>
       <c r="V10" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W10" t="s">
         <v>29</v>
       </c>
       <c r="X10" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y10" t="s">
         <v>29</v>
@@ -2248,28 +2257,28 @@
         <v>30</v>
       </c>
       <c r="Q11" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R11" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S11" t="s">
         <v>29</v>
       </c>
       <c r="T11" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U11" t="s">
         <v>30</v>
       </c>
       <c r="V11" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W11" t="s">
         <v>38</v>
       </c>
       <c r="X11" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y11" t="s">
         <v>29</v>
@@ -2323,28 +2332,28 @@
         <v>29</v>
       </c>
       <c r="Q12" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R12" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S12" t="s">
         <v>30</v>
       </c>
       <c r="T12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U12" t="s">
         <v>30</v>
       </c>
       <c r="V12" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W12" t="s">
         <v>38</v>
       </c>
       <c r="X12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y12" t="s">
         <v>29</v>
@@ -2370,7 +2379,7 @@
         <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>30</v>
@@ -2400,10 +2409,10 @@
         <v>30</v>
       </c>
       <c r="Q13" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R13" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S13" t="s">
         <v>29</v>
@@ -2415,13 +2424,13 @@
         <v>30</v>
       </c>
       <c r="V13" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W13" t="s">
         <v>38</v>
       </c>
       <c r="X13" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y13" t="s">
         <v>29</v>
@@ -2447,7 +2456,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>30</v>
@@ -2475,28 +2484,28 @@
         <v>30</v>
       </c>
       <c r="Q14" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R14" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S14" t="s">
         <v>29</v>
       </c>
       <c r="T14" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U14" t="s">
         <v>30</v>
       </c>
       <c r="V14" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W14" t="s">
         <v>38</v>
       </c>
       <c r="X14" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y14" t="s">
         <v>29</v>
@@ -2550,28 +2559,28 @@
         <v>30</v>
       </c>
       <c r="Q15" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R15" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S15" t="s">
         <v>29</v>
       </c>
       <c r="T15" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U15" t="s">
         <v>30</v>
       </c>
       <c r="V15" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W15" t="s">
         <v>38</v>
       </c>
       <c r="X15" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y15" t="s">
         <v>29</v>
@@ -2625,28 +2634,28 @@
         <v>29</v>
       </c>
       <c r="Q16" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S16" t="s">
         <v>29</v>
       </c>
       <c r="T16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U16" t="s">
         <v>29</v>
       </c>
       <c r="V16" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W16" t="s">
         <v>38</v>
       </c>
       <c r="X16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y16" t="s">
         <v>29</v>
@@ -2696,22 +2705,22 @@
         <v>27</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="P17" t="s">
         <v>29</v>
       </c>
       <c r="Q17" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S17" t="s">
         <v>30</v>
       </c>
       <c r="T17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U17" t="s">
         <v>29</v>
@@ -2723,7 +2732,7 @@
         <v>29</v>
       </c>
       <c r="X17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y17" t="s">
         <v>29</v>
@@ -2758,7 +2767,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5">
         <v>35</v>
@@ -2775,10 +2784,10 @@
         <v>30</v>
       </c>
       <c r="Q18" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R18" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S18" t="s">
         <v>29</v>
@@ -2790,13 +2799,13 @@
         <v>30</v>
       </c>
       <c r="V18" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W18" t="s">
         <v>38</v>
       </c>
       <c r="X18" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y18" t="s">
         <v>30</v>
@@ -2831,7 +2840,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K19" s="5">
         <v>45</v>
@@ -2850,16 +2859,16 @@
         <v>29</v>
       </c>
       <c r="Q19" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R19" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S19" t="s">
         <v>29</v>
       </c>
       <c r="T19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U19" t="s">
         <v>29</v>
@@ -2871,7 +2880,7 @@
         <v>38</v>
       </c>
       <c r="X19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y19" t="s">
         <v>29</v>
@@ -2921,34 +2930,34 @@
         <v>49</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="P20" t="s">
         <v>30</v>
       </c>
       <c r="Q20" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R20" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S20" t="s">
         <v>29</v>
       </c>
       <c r="T20" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U20" t="s">
         <v>30</v>
       </c>
       <c r="V20" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W20" t="s">
         <v>29</v>
       </c>
       <c r="X20" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y20" t="s">
         <v>29</v>
@@ -3002,16 +3011,16 @@
         <v>29</v>
       </c>
       <c r="Q21" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R21" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S21" t="s">
         <v>29</v>
       </c>
       <c r="T21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U21" t="s">
         <v>29</v>
@@ -3023,7 +3032,7 @@
         <v>38</v>
       </c>
       <c r="X21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y21" t="s">
         <v>29</v>
@@ -3058,7 +3067,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="K22" s="5">
         <v>55</v>
@@ -3077,16 +3086,16 @@
         <v>29</v>
       </c>
       <c r="Q22" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R22" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S22" t="s">
         <v>29</v>
       </c>
       <c r="T22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U22" t="s">
         <v>29</v>
@@ -3098,7 +3107,7 @@
         <v>29</v>
       </c>
       <c r="X22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y22" t="s">
         <v>29</v>
@@ -3150,16 +3159,16 @@
         <v>29</v>
       </c>
       <c r="Q23" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R23" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S23" t="s">
         <v>29</v>
       </c>
       <c r="T23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U23" t="s">
         <v>29</v>
@@ -3171,7 +3180,7 @@
         <v>29</v>
       </c>
       <c r="X23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y23" t="s">
         <v>29</v>
@@ -3206,7 +3215,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K24" s="5">
         <v>48</v>
@@ -3223,28 +3232,28 @@
         <v>29</v>
       </c>
       <c r="Q24" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S24" t="s">
         <v>29</v>
       </c>
       <c r="T24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U24" t="s">
         <v>29</v>
       </c>
       <c r="V24" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W24" t="s">
         <v>29</v>
       </c>
       <c r="X24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y24" t="s">
         <v>29</v>
@@ -3279,7 +3288,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K25" s="5">
         <v>30</v>
@@ -3296,28 +3305,28 @@
         <v>30</v>
       </c>
       <c r="Q25" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R25" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S25" t="s">
         <v>29</v>
       </c>
       <c r="T25" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U25" t="s">
         <v>30</v>
       </c>
       <c r="V25" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W25" t="s">
         <v>29</v>
       </c>
       <c r="X25" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y25" t="s">
         <v>29</v>
@@ -3352,7 +3361,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="K26" s="5">
         <v>55</v>
@@ -3364,35 +3373,35 @@
         <v>0.88</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s">
         <v>29</v>
       </c>
       <c r="Q26" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S26" t="s">
         <v>29</v>
       </c>
       <c r="T26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U26" t="s">
         <v>30</v>
       </c>
       <c r="V26" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W26" t="s">
         <v>29</v>
       </c>
       <c r="X26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y26" t="s">
         <v>29</v>
@@ -3427,7 +3436,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="K27" s="5">
         <v>43</v>
@@ -3439,17 +3448,17 @@
         <v>0.61</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s">
         <v>29</v>
       </c>
       <c r="Q27" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R27" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S27" t="s">
         <v>29</v>
@@ -3461,13 +3470,13 @@
         <v>29</v>
       </c>
       <c r="V27" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="W27" t="s">
         <v>29</v>
       </c>
       <c r="X27" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y27" t="s">
         <v>29</v>
@@ -3484,7 +3493,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="E28" s="5">
         <v>30.5</v>
@@ -3502,7 +3511,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K28" s="5">
         <v>44</v>
@@ -3521,10 +3530,10 @@
         <v>30</v>
       </c>
       <c r="Q28" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="R28" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S28" t="s">
         <v>30</v>
@@ -3536,13 +3545,13 @@
         <v>30</v>
       </c>
       <c r="V28" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W28" t="s">
         <v>30</v>
       </c>
       <c r="X28" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y28" t="s">
         <v>29</v>
@@ -3577,7 +3586,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="K29" s="5">
         <v>39</v>
@@ -3589,35 +3598,35 @@
         <v>0.65</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s">
         <v>29</v>
       </c>
       <c r="Q29" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R29" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S29" t="s">
         <v>29</v>
       </c>
       <c r="T29" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U29" t="s">
         <v>29</v>
       </c>
       <c r="V29" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W29" t="s">
         <v>29</v>
       </c>
       <c r="X29" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y29" t="s">
         <v>29</v>
@@ -3669,28 +3678,28 @@
         <v>29</v>
       </c>
       <c r="Q30" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R30" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S30" t="s">
         <v>29</v>
       </c>
       <c r="T30" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U30" t="s">
         <v>29</v>
       </c>
       <c r="V30" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W30" t="s">
         <v>38</v>
       </c>
       <c r="X30" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y30" t="s">
         <v>29</v>
@@ -3725,7 +3734,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -3742,28 +3751,28 @@
         <v>30</v>
       </c>
       <c r="Q31" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R31" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="S31" t="s">
         <v>29</v>
       </c>
       <c r="T31" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U31" t="s">
         <v>30</v>
       </c>
       <c r="V31" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W31" t="s">
         <v>38</v>
       </c>
       <c r="X31" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y31" t="s">
         <v>29</v>
@@ -3798,7 +3807,7 @@
         <v>10</v>
       </c>
       <c r="J32" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K32" s="5">
         <v>36</v>
@@ -3815,28 +3824,28 @@
         <v>29</v>
       </c>
       <c r="Q32" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="R32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="S32" t="s">
         <v>29</v>
       </c>
       <c r="T32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U32" t="s">
         <v>30</v>
       </c>
       <c r="V32" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W32" t="s">
         <v>29</v>
       </c>
       <c r="X32" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y32" t="s">
         <v>29</v>
@@ -3888,28 +3897,28 @@
         <v>30</v>
       </c>
       <c r="Q33" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="R33" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S33" t="s">
         <v>29</v>
       </c>
       <c r="T33" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="U33" t="s">
         <v>30</v>
       </c>
       <c r="V33" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W33" t="s">
         <v>30</v>
       </c>
       <c r="X33" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y33" t="s">
         <v>29</v>
@@ -3961,16 +3970,16 @@
         <v>29</v>
       </c>
       <c r="Q34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="R34" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S34" t="s">
         <v>29</v>
       </c>
       <c r="T34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U34" t="s">
         <v>29</v>
@@ -3982,7 +3991,7 @@
         <v>29</v>
       </c>
       <c r="X34" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y34" t="s">
         <v>29</v>
@@ -4017,7 +4026,7 @@
         <v>9</v>
       </c>
       <c r="J35" s="5" t="s">
-        <v>182</v>
+        <v>107</v>
       </c>
       <c r="K35" s="5">
         <v>25</v>
@@ -4029,62 +4038,344 @@
         <v>0.8</v>
       </c>
       <c r="N35" s="7" t="s">
-        <v>183</v>
+        <v>108</v>
       </c>
       <c r="O35" s="2"/>
       <c r="P35" t="s">
         <v>30</v>
       </c>
       <c r="Q35" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="R35" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="S35" t="s">
         <v>29</v>
       </c>
       <c r="T35" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="U35" t="s">
         <v>30</v>
       </c>
       <c r="V35" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
       <c r="W35" t="s">
         <v>38</v>
       </c>
       <c r="X35" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Y35" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:25" x14ac:dyDescent="0.3">
-      <c r="B36" s="1"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="5"/>
-      <c r="E36" s="5"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="6"/>
-      <c r="H36" s="5"/>
-      <c r="I36" s="5"/>
-      <c r="J36" s="5"/>
-      <c r="K36" s="5"/>
-      <c r="L36" s="5"/>
-      <c r="M36" s="7"/>
+      <c r="A36" t="s">
+        <v>43</v>
+      </c>
+      <c r="B36" s="1">
+        <v>43830</v>
+      </c>
+      <c r="C36" s="4">
+        <v>8.3333333333333329E-2</v>
+      </c>
+      <c r="D36" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5">
+        <v>2</v>
+      </c>
+      <c r="F36" s="6">
+        <v>22</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H36" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I36" s="5">
+        <v>9</v>
+      </c>
+      <c r="J36" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="K36" s="5">
+        <v>45</v>
+      </c>
+      <c r="L36" s="5">
+        <v>41</v>
+      </c>
+      <c r="M36" s="7">
+        <v>0.86</v>
+      </c>
       <c r="N36" s="7"/>
       <c r="O36" s="2"/>
+      <c r="P36" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>88</v>
+      </c>
+      <c r="R36" t="s">
+        <v>82</v>
+      </c>
+      <c r="S36" t="s">
+        <v>29</v>
+      </c>
+      <c r="T36" t="s">
+        <v>82</v>
+      </c>
+      <c r="U36" t="s">
+        <v>29</v>
+      </c>
+      <c r="V36" t="s">
+        <v>20</v>
+      </c>
+      <c r="W36" t="s">
+        <v>29</v>
+      </c>
+      <c r="X36" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>43</v>
+      </c>
+      <c r="B37" s="1">
+        <v>43466</v>
+      </c>
+      <c r="C37" s="4">
+        <v>0.375</v>
+      </c>
+      <c r="D37" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E37" s="5">
+        <v>5.5</v>
+      </c>
+      <c r="F37" s="6">
+        <v>60</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="H37" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I37" s="5">
+        <v>9</v>
+      </c>
+      <c r="J37" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="K37" s="5">
+        <v>28</v>
+      </c>
+      <c r="L37" s="5">
+        <v>20</v>
+      </c>
+      <c r="M37" s="7">
+        <v>1</v>
+      </c>
+      <c r="N37" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O37" s="2"/>
+      <c r="P37" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>82</v>
+      </c>
+      <c r="R37" t="s">
+        <v>88</v>
+      </c>
+      <c r="S37" t="s">
+        <v>29</v>
+      </c>
+      <c r="T37" t="s">
+        <v>103</v>
+      </c>
+      <c r="U37" t="s">
+        <v>30</v>
+      </c>
+      <c r="V37" t="s">
+        <v>93</v>
+      </c>
+      <c r="W37" t="s">
+        <v>38</v>
+      </c>
+      <c r="X37" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="38" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="1">
+        <v>43468</v>
+      </c>
+      <c r="C38" s="4">
+        <v>0.41666666666666669</v>
+      </c>
+      <c r="D38" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E38" s="5">
+        <v>3.5</v>
+      </c>
+      <c r="F38" s="6">
+        <v>40</v>
+      </c>
+      <c r="G38" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H38" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I38" s="5">
+        <v>8</v>
+      </c>
+      <c r="J38" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K38" s="5">
+        <v>37</v>
+      </c>
+      <c r="L38" s="5">
+        <v>32</v>
+      </c>
+      <c r="M38" s="7">
+        <v>0.87</v>
+      </c>
+      <c r="N38" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O38" s="2"/>
+      <c r="P38" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>89</v>
+      </c>
+      <c r="R38" t="s">
+        <v>87</v>
+      </c>
+      <c r="S38" t="s">
+        <v>29</v>
+      </c>
+      <c r="T38" t="s">
+        <v>82</v>
+      </c>
+      <c r="U38" t="s">
+        <v>30</v>
+      </c>
+      <c r="V38" t="s">
+        <v>94</v>
+      </c>
+      <c r="W38" t="s">
+        <v>29</v>
+      </c>
+      <c r="X38" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="39" spans="1:25" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>43</v>
+      </c>
+      <c r="B39" s="1">
+        <v>43470</v>
+      </c>
+      <c r="C39" s="4">
+        <v>0.29166666666666669</v>
+      </c>
+      <c r="D39" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="E39" s="5">
+        <v>7.5</v>
+      </c>
+      <c r="F39" s="6">
+        <v>80</v>
+      </c>
+      <c r="G39" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="H39" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="I39" s="5">
+        <v>5</v>
+      </c>
+      <c r="J39" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="K39" s="5">
+        <v>30</v>
+      </c>
+      <c r="L39" s="5">
+        <v>30</v>
+      </c>
+      <c r="M39" s="7">
+        <v>1</v>
+      </c>
+      <c r="N39" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="O39" s="2"/>
+      <c r="P39" t="s">
+        <v>29</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>88</v>
+      </c>
+      <c r="R39" t="s">
+        <v>87</v>
+      </c>
+      <c r="S39" t="s">
+        <v>29</v>
+      </c>
+      <c r="T39" t="s">
+        <v>82</v>
+      </c>
+      <c r="U39" t="s">
+        <v>30</v>
+      </c>
+      <c r="V39" t="s">
+        <v>96</v>
+      </c>
+      <c r="W39" t="s">
+        <v>29</v>
+      </c>
+      <c r="X39" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>29</v>
+      </c>
     </row>
   </sheetData>
   <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G36" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G2:G39" xr:uid="{796A7D2B-6F7A-406E-A1B0-4534F3804EBB}">
       <formula1>Conditions</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T36" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T2:T39" xr:uid="{D6029D36-E4DB-48BF-A564-DF5B1EB29061}">
       <formula1>JacketOption</formula1>
     </dataValidation>
   </dataValidations>
@@ -4100,25 +4391,25 @@
           <x14:formula1>
             <xm:f>ValidValues!$C$2:$C$3</xm:f>
           </x14:formula1>
-          <xm:sqref>P2:P36 S2:S36 U2:U36 W2:W36 Y2:Y36</xm:sqref>
+          <xm:sqref>P2:P39 S2:S39 U2:U39 W2:W39 Y2:Y39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{4BFEBF07-64B2-450B-BC13-447B52D5D711}">
           <x14:formula1>
             <xm:f>ValidValues!$G$2:$G$6</xm:f>
           </x14:formula1>
-          <xm:sqref>Q2:R36</xm:sqref>
+          <xm:sqref>Q2:R39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{8E09EE0F-16F0-4536-B318-2F013ED3F6AB}">
           <x14:formula1>
             <xm:f>ValidValues!$I$2:$I$6</xm:f>
           </x14:formula1>
-          <xm:sqref>V2:V36</xm:sqref>
+          <xm:sqref>V2:V39</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{1617D946-B125-4BE6-B340-3AE6EE661815}">
           <x14:formula1>
             <xm:f>ValidValues!$J$2:$J$4</xm:f>
           </x14:formula1>
-          <xm:sqref>X2:X36</xm:sqref>
+          <xm:sqref>X2:X39</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -4165,7 +4456,7 @@
         <v>6</v>
       </c>
       <c r="G1" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="H1" t="s">
         <v>32</v>
@@ -4231,7 +4522,7 @@
         <v>50</v>
       </c>
       <c r="AC1" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:32" x14ac:dyDescent="0.3">
@@ -4306,7 +4597,7 @@
         <v>30</v>
       </c>
       <c r="Y2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z2" t="s">
         <v>30</v>
@@ -4393,7 +4684,7 @@
         <v>30</v>
       </c>
       <c r="Y3" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z3" t="s">
         <v>30</v>
@@ -4412,7 +4703,7 @@
       </c>
       <c r="AF3">
         <f ca="1">RANDBETWEEN(0,100)</f>
-        <v>77</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.3">
@@ -4487,7 +4778,7 @@
         <v>30</v>
       </c>
       <c r="Y4" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z4" t="s">
         <v>29</v>
@@ -4506,7 +4797,7 @@
       </c>
       <c r="AF4">
         <f ca="1">RANDBETWEEN(0,20)</f>
-        <v>6</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" spans="1:32" x14ac:dyDescent="0.3">
@@ -4581,7 +4872,7 @@
         <v>30</v>
       </c>
       <c r="Y5" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z5" t="s">
         <v>29</v>
@@ -4600,7 +4891,7 @@
       </c>
       <c r="AF5">
         <f ca="1">RANDBETWEEN(35,95)</f>
-        <v>58</v>
+        <v>74</v>
       </c>
     </row>
     <row r="6" spans="1:32" x14ac:dyDescent="0.3">
@@ -4677,7 +4968,7 @@
         <v>30</v>
       </c>
       <c r="Y6" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z6" t="s">
         <v>29</v>
@@ -4764,7 +5055,7 @@
         <v>30</v>
       </c>
       <c r="Y7" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z7" t="s">
         <v>30</v>
@@ -4851,7 +5142,7 @@
         <v>29</v>
       </c>
       <c r="Y8" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z8" t="s">
         <v>29</v>
@@ -4938,7 +5229,7 @@
         <v>30</v>
       </c>
       <c r="Y9" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z9" t="s">
         <v>29</v>
@@ -5025,7 +5316,7 @@
         <v>29</v>
       </c>
       <c r="Y10" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z10" t="s">
         <v>29</v>
@@ -5112,7 +5403,7 @@
         <v>29</v>
       </c>
       <c r="Y11" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z11" t="s">
         <v>29</v>
@@ -5199,7 +5490,7 @@
         <v>30</v>
       </c>
       <c r="Y12" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z12" t="s">
         <v>30</v>
@@ -5234,7 +5525,7 @@
         <v>70</v>
       </c>
       <c r="G13" s="6" t="s">
-        <v>116</v>
+        <v>66</v>
       </c>
       <c r="H13" s="5" t="s">
         <v>30</v>
@@ -5288,7 +5579,7 @@
         <v>29</v>
       </c>
       <c r="Y13" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z13" t="s">
         <v>29</v>
@@ -5323,7 +5614,7 @@
         <v>32</v>
       </c>
       <c r="G14" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="H14" s="5" t="s">
         <v>30</v>
@@ -5375,7 +5666,7 @@
         <v>29</v>
       </c>
       <c r="Y14" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z14" t="s">
         <v>29</v>
@@ -5462,7 +5753,7 @@
         <v>29</v>
       </c>
       <c r="Y15" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z15" t="s">
         <v>29</v>
@@ -5549,7 +5840,7 @@
         <v>30</v>
       </c>
       <c r="Y16" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z16" t="s">
         <v>30</v>
@@ -5608,7 +5899,7 @@
         <v>27</v>
       </c>
       <c r="O17" s="2" t="s">
-        <v>142</v>
+        <v>67</v>
       </c>
       <c r="P17" t="s">
         <v>29</v>
@@ -5638,7 +5929,7 @@
         <v>30</v>
       </c>
       <c r="Y17" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z17" t="s">
         <v>29</v>
@@ -5682,7 +5973,7 @@
         <v>2</v>
       </c>
       <c r="J18" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K18" s="5">
         <v>35</v>
@@ -5723,7 +6014,7 @@
         <v>29</v>
       </c>
       <c r="Y18" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z18" t="s">
         <v>29</v>
@@ -5767,7 +6058,7 @@
         <v>5</v>
       </c>
       <c r="J19" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K19" s="5">
         <v>45</v>
@@ -5810,7 +6101,7 @@
         <v>30</v>
       </c>
       <c r="Y19" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z19" t="s">
         <v>29</v>
@@ -5869,7 +6160,7 @@
         <v>49</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>146</v>
+        <v>71</v>
       </c>
       <c r="P20" t="s">
         <v>29</v>
@@ -5899,7 +6190,7 @@
         <v>29</v>
       </c>
       <c r="Y20" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z20" t="s">
         <v>29</v>
@@ -5986,7 +6277,7 @@
         <v>30</v>
       </c>
       <c r="Y21" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z21" t="s">
         <v>29</v>
@@ -6030,7 +6321,7 @@
         <v>12</v>
       </c>
       <c r="J22" s="5" t="s">
-        <v>147</v>
+        <v>72</v>
       </c>
       <c r="K22" s="5">
         <v>55</v>
@@ -6073,7 +6364,7 @@
         <v>30</v>
       </c>
       <c r="Y22" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z22" t="s">
         <v>29</v>
@@ -6158,7 +6449,7 @@
         <v>30</v>
       </c>
       <c r="Y23" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z23" t="s">
         <v>29</v>
@@ -6202,7 +6493,7 @@
         <v>23</v>
       </c>
       <c r="J24" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K24" s="5">
         <v>48</v>
@@ -6243,7 +6534,7 @@
         <v>30</v>
       </c>
       <c r="Y24" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z24" t="s">
         <v>30</v>
@@ -6287,7 +6578,7 @@
         <v>3</v>
       </c>
       <c r="J25" s="5" t="s">
-        <v>145</v>
+        <v>70</v>
       </c>
       <c r="K25" s="5">
         <v>30</v>
@@ -6328,7 +6619,7 @@
         <v>29</v>
       </c>
       <c r="Y25" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z25" t="s">
         <v>29</v>
@@ -6372,7 +6663,7 @@
         <v>5</v>
       </c>
       <c r="J26" s="5" t="s">
-        <v>149</v>
+        <v>74</v>
       </c>
       <c r="K26" s="5">
         <v>55</v>
@@ -6384,7 +6675,7 @@
         <v>0.88</v>
       </c>
       <c r="N26" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s">
@@ -6415,7 +6706,7 @@
         <v>30</v>
       </c>
       <c r="Y26" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z26" t="s">
         <v>30</v>
@@ -6459,7 +6750,7 @@
         <v>13</v>
       </c>
       <c r="J27" s="5" t="s">
-        <v>151</v>
+        <v>76</v>
       </c>
       <c r="K27" s="5">
         <v>43</v>
@@ -6471,7 +6762,7 @@
         <v>0.61</v>
       </c>
       <c r="N27" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s">
@@ -6502,7 +6793,7 @@
         <v>30</v>
       </c>
       <c r="Y27" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="Z27" t="s">
         <v>30</v>
@@ -6528,7 +6819,7 @@
         <v>4.1666666666666664E-2</v>
       </c>
       <c r="D28" s="5" t="s">
-        <v>152</v>
+        <v>77</v>
       </c>
       <c r="E28" s="5">
         <v>30.5</v>
@@ -6546,7 +6837,7 @@
         <v>16</v>
       </c>
       <c r="J28" s="5" t="s">
-        <v>144</v>
+        <v>69</v>
       </c>
       <c r="K28" s="5">
         <v>44</v>
@@ -6589,7 +6880,7 @@
         <v>29</v>
       </c>
       <c r="Y28" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z28" t="s">
         <v>29</v>
@@ -6633,7 +6924,7 @@
         <v>9</v>
       </c>
       <c r="J29" s="5" t="s">
-        <v>158</v>
+        <v>83</v>
       </c>
       <c r="K29" s="5">
         <v>39</v>
@@ -6645,7 +6936,7 @@
         <v>0.65</v>
       </c>
       <c r="N29" s="7" t="s">
-        <v>150</v>
+        <v>75</v>
       </c>
       <c r="O29" s="2"/>
       <c r="P29" t="s">
@@ -6676,7 +6967,7 @@
         <v>29</v>
       </c>
       <c r="Y29" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z29" t="s">
         <v>29</v>
@@ -6761,7 +7052,7 @@
         <v>29</v>
       </c>
       <c r="Y30" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z30" t="s">
         <v>29</v>
@@ -6805,7 +7096,7 @@
         <v>5</v>
       </c>
       <c r="J31" s="5" t="s">
-        <v>173</v>
+        <v>98</v>
       </c>
       <c r="K31" s="5">
         <v>37</v>
@@ -6846,7 +7137,7 @@
         <v>29</v>
       </c>
       <c r="Y31" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="Z31" t="s">
         <v>29</v>
@@ -6913,8 +7204,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CF5CF31-5DCF-45F0-99A9-605CADC9A594}">
   <dimension ref="A1:J94"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+    <sheetView topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5:A94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -6931,22 +7222,22 @@
         <v>7</v>
       </c>
       <c r="C1" t="s">
-        <v>153</v>
+        <v>78</v>
       </c>
       <c r="E1" t="s">
         <v>21</v>
       </c>
       <c r="G1" t="s">
-        <v>161</v>
+        <v>86</v>
       </c>
       <c r="H1" t="s">
         <v>18</v>
       </c>
       <c r="I1" t="s">
-        <v>170</v>
+        <v>95</v>
       </c>
       <c r="J1" t="s">
-        <v>175</v>
+        <v>100</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.3">
@@ -6957,19 +7248,19 @@
         <v>30</v>
       </c>
       <c r="E2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="G2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="H2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
       <c r="I2" t="s">
         <v>20</v>
       </c>
       <c r="J2" t="s">
-        <v>157</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.3">
@@ -6980,19 +7271,19 @@
         <v>29</v>
       </c>
       <c r="E3" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="G3" t="s">
-        <v>160</v>
+        <v>85</v>
       </c>
       <c r="H3" t="s">
-        <v>178</v>
+        <v>103</v>
       </c>
       <c r="I3" t="s">
-        <v>171</v>
+        <v>96</v>
       </c>
       <c r="J3" t="s">
-        <v>176</v>
+        <v>101</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.3">
@@ -7000,237 +7291,237 @@
         <v>109</v>
       </c>
       <c r="E4" t="s">
-        <v>155</v>
+        <v>80</v>
       </c>
       <c r="G4" t="s">
-        <v>162</v>
+        <v>87</v>
       </c>
       <c r="H4" t="s">
-        <v>165</v>
+        <v>90</v>
       </c>
       <c r="I4" t="s">
-        <v>154</v>
+        <v>79</v>
       </c>
       <c r="J4" t="s">
-        <v>177</v>
+        <v>102</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="E5" t="s">
-        <v>156</v>
+        <v>81</v>
       </c>
       <c r="G5" t="s">
-        <v>163</v>
+        <v>88</v>
       </c>
       <c r="H5" t="s">
         <v>39</v>
       </c>
       <c r="I5" t="s">
-        <v>168</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>107</v>
+        <v>111</v>
       </c>
       <c r="G6" t="s">
-        <v>164</v>
+        <v>89</v>
       </c>
       <c r="H6" t="s">
         <v>8</v>
       </c>
       <c r="I6" t="s">
-        <v>169</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>95</v>
+        <v>112</v>
       </c>
       <c r="H7" t="s">
-        <v>166</v>
+        <v>91</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>79</v>
+        <v>113</v>
       </c>
       <c r="H8" t="s">
-        <v>179</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>81</v>
+        <v>114</v>
       </c>
       <c r="H9" t="s">
-        <v>180</v>
+        <v>105</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>137</v>
+        <v>115</v>
       </c>
       <c r="H10" t="s">
-        <v>181</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>141</v>
+        <v>116</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>139</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>91</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
     </row>
     <row r="17" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
     </row>
     <row r="18" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>73</v>
+        <v>123</v>
       </c>
     </row>
     <row r="19" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>124</v>
       </c>
     </row>
     <row r="20" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>99</v>
+        <v>125</v>
       </c>
     </row>
     <row r="21" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>101</v>
+        <v>126</v>
       </c>
     </row>
     <row r="22" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>127</v>
       </c>
     </row>
     <row r="23" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
     </row>
     <row r="24" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>111</v>
+        <v>129</v>
       </c>
     </row>
     <row r="25" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
     </row>
     <row r="26" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>89</v>
+        <v>131</v>
       </c>
     </row>
     <row r="27" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>132</v>
       </c>
     </row>
     <row r="28" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
-        <v>123</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
     </row>
     <row r="30" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
-        <v>67</v>
+        <v>135</v>
       </c>
     </row>
     <row r="31" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
     </row>
     <row r="32" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
-        <v>69</v>
+        <v>137</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
-        <v>115</v>
+        <v>138</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
-        <v>93</v>
+        <v>139</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>131</v>
+        <v>141</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>143</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>133</v>
+        <v>144</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>135</v>
+        <v>145</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>146</v>
       </c>
       <c r="C41" s="3" t="s">
         <v>51</v>
@@ -7238,7 +7529,7 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
-        <v>87</v>
+        <v>147</v>
       </c>
       <c r="C42" s="3" t="s">
         <v>52</v>
@@ -7254,7 +7545,7 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
-        <v>108</v>
+        <v>148</v>
       </c>
       <c r="C44" s="3" t="s">
         <v>54</v>
@@ -7262,7 +7553,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
-        <v>104</v>
+        <v>149</v>
       </c>
       <c r="C45" s="3" t="s">
         <v>35</v>
@@ -7270,7 +7561,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
-        <v>106</v>
+        <v>150</v>
       </c>
       <c r="C46" s="3" t="s">
         <v>31</v>
@@ -7278,7 +7569,7 @@
     </row>
     <row r="47" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
-        <v>94</v>
+        <v>151</v>
       </c>
       <c r="C47" s="3" t="s">
         <v>55</v>
@@ -7286,7 +7577,7 @@
     </row>
     <row r="48" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
-        <v>78</v>
+        <v>152</v>
       </c>
       <c r="C48" s="3" t="s">
         <v>56</v>
@@ -7294,7 +7585,7 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
-        <v>80</v>
+        <v>153</v>
       </c>
       <c r="C49" s="3" t="s">
         <v>57</v>
@@ -7302,7 +7593,7 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
-        <v>136</v>
+        <v>154</v>
       </c>
       <c r="C50" s="3" t="s">
         <v>58</v>
@@ -7310,7 +7601,7 @@
     </row>
     <row r="51" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="C51" s="3" t="s">
         <v>59</v>
@@ -7318,7 +7609,7 @@
     </row>
     <row r="52" spans="1:3" ht="19.2" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
-        <v>138</v>
+        <v>156</v>
       </c>
       <c r="C52" s="3" t="s">
         <v>60</v>
@@ -7326,7 +7617,7 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A53" t="s">
-        <v>74</v>
+        <v>157</v>
       </c>
       <c r="C53" s="3" t="s">
         <v>61</v>
@@ -7334,147 +7625,147 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>90</v>
+        <v>159</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>70</v>
+        <v>160</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
-        <v>118</v>
+        <v>161</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
-        <v>72</v>
+        <v>162</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
-        <v>102</v>
+        <v>163</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
-        <v>98</v>
+        <v>164</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
-        <v>100</v>
+        <v>165</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
-        <v>76</v>
+        <v>166</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
-        <v>64</v>
+        <v>167</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
-        <v>110</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
-        <v>112</v>
+        <v>169</v>
       </c>
     </row>
     <row r="66" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
-        <v>88</v>
+        <v>170</v>
       </c>
     </row>
     <row r="67" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
-        <v>96</v>
+        <v>171</v>
       </c>
     </row>
     <row r="68" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>172</v>
       </c>
     </row>
     <row r="69" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
-        <v>82</v>
+        <v>173</v>
       </c>
     </row>
     <row r="70" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
-        <v>66</v>
+        <v>174</v>
       </c>
     </row>
     <row r="71" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
-        <v>116</v>
+        <v>175</v>
       </c>
     </row>
     <row r="72" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
-        <v>68</v>
+        <v>176</v>
       </c>
     </row>
     <row r="73" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
-        <v>114</v>
+        <v>177</v>
       </c>
     </row>
     <row r="74" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
-        <v>92</v>
+        <v>178</v>
       </c>
     </row>
     <row r="75" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A75" t="s">
-        <v>124</v>
+        <v>179</v>
       </c>
     </row>
     <row r="76" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
-        <v>130</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
-        <v>126</v>
+        <v>181</v>
       </c>
     </row>
     <row r="78" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
-        <v>128</v>
+        <v>182</v>
       </c>
     </row>
     <row r="79" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
-        <v>132</v>
+        <v>183</v>
       </c>
     </row>
     <row r="80" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
-        <v>134</v>
+        <v>184</v>
       </c>
     </row>
     <row r="81" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
-        <v>84</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:1" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
-        <v>86</v>
+        <v>186</v>
       </c>
     </row>
     <row r="83" spans="1:1" x14ac:dyDescent="0.3">
@@ -7579,7 +7870,7 @@
         <v>6</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>148</v>
+        <v>73</v>
       </c>
       <c r="E1" s="9" t="s">
         <v>32</v>
@@ -7648,7 +7939,7 @@
         <v>50</v>
       </c>
       <c r="AA1" s="10" t="s">
-        <v>143</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:27" x14ac:dyDescent="0.3">

</xml_diff>